<commit_message>
added async and shortid
</commit_message>
<xml_diff>
--- a/experiments/AlgoComparisons.xlsx
+++ b/experiments/AlgoComparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\mutode_research\newDD\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90716A88-59A9-4AD0-9D34-037B68E9ECDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233F351C-94A7-4048-AA02-6A705E28265D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2801" yWindow="2801" windowWidth="18851" windowHeight="9845" xr2:uid="{1807BA8C-4E5D-4B92-917C-C9945C819F91}"/>
+    <workbookView xWindow="2239" yWindow="2239" windowWidth="18850" windowHeight="9844" xr2:uid="{1807BA8C-4E5D-4B92-917C-C9945C819F91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="166">
   <si>
     <t>ddMin</t>
   </si>
@@ -410,15 +410,6 @@
     <t>4h 12.9s</t>
   </si>
   <si>
-    <t>socket.io@2.1.0</t>
-  </si>
-  <si>
-    <t>0-22</t>
-  </si>
-  <si>
-    <t>25s</t>
-  </si>
-  <si>
     <t>passport@0.4.1</t>
   </si>
   <si>
@@ -485,10 +476,67 @@
     <t>Date of Experiment</t>
   </si>
   <si>
-    <t>10/17/2020</t>
-  </si>
-  <si>
-    <t>Issues with this experiment, irregular test case output</t>
+    <t>shortid@2.2.16</t>
+  </si>
+  <si>
+    <t>27m 59s</t>
+  </si>
+  <si>
+    <t>2s</t>
+  </si>
+  <si>
+    <t>0-16</t>
+  </si>
+  <si>
+    <t>64ms</t>
+  </si>
+  <si>
+    <t>2,3,7</t>
+  </si>
+  <si>
+    <t>226ms</t>
+  </si>
+  <si>
+    <t>57ms</t>
+  </si>
+  <si>
+    <t>3,2,6</t>
+  </si>
+  <si>
+    <t>347ms</t>
+  </si>
+  <si>
+    <t>849ms</t>
+  </si>
+  <si>
+    <t>async@2.6.0</t>
+  </si>
+  <si>
+    <t>0-510</t>
+  </si>
+  <si>
+    <t>6h 51m</t>
+  </si>
+  <si>
+    <t>18s</t>
+  </si>
+  <si>
+    <t>3s 856ms</t>
+  </si>
+  <si>
+    <t>128,130,133,140,142,259,262,263,271,273,279,280,282,283,284,304,305,306,310,336,338,339,340,343,346,347,348,354,356,361,365,371,375,376,382,384,386,387,388,390,395,396,399,400,402,404,406,407,416,419,420,421,422,423,424,433,434,441,443,444,463,469,470,472,476,479,482,483,489,493,494,496,497,499,500</t>
+  </si>
+  <si>
+    <t>1s 140ms</t>
+  </si>
+  <si>
+    <t>483,104,416,501,201,338,55,424,293,194,269,17,119,423,280,408,461,387,175,497,365,272,193,394,382,2,302,258,43,262,164,396,133,252,251,422,430,448,301,473,180,341,146,111,391,124,0,184,392,343,56,373,489,476,177,506,80,375,238,58,367,406,508,95,191,166,309,102,295,134,199,140,432,463,493,101,339,400,304,172,356</t>
+  </si>
+  <si>
+    <t>398ms</t>
+  </si>
+  <si>
+    <t>Note : The mutation scores qouted above are not what the original tool returned, those can be calculated by the killed,survived, discarded mutant given ahead. However this mutation score is computed after we discard a few more mutants, that we not valid for analysis (for example entire test suite failed due to compilation error introduced by a mutation)</t>
   </si>
 </sst>
 </file>
@@ -699,7 +747,7 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -760,9 +808,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1067,7 +1112,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{750652E7-E767-41D1-9927-FDCE55E1E6D0}" name="Table12" displayName="Table12" ref="D1:M23" totalsRowShown="0" headerRowDxfId="18" headerRowCellStyle="Neutral">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{750652E7-E767-41D1-9927-FDCE55E1E6D0}" name="Table12" displayName="Table12" ref="D1:M24" totalsRowShown="0" headerRowDxfId="18" headerRowCellStyle="Neutral">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{15CF07D5-B71B-4A28-8125-12ACDB9CC697}" name="Original Set" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{0D187438-7867-4CF4-BC39-4C5405F1DE55}" name="Mutation Score" dataDxfId="16"/>
@@ -1395,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A84B95-A035-4AC9-8702-F9EE4E2D8975}">
-  <dimension ref="A1:AQ23"/>
+  <dimension ref="A1:AQ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AL12" sqref="AL12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1442,10 +1487,10 @@
   <sheetData>
     <row r="1" spans="1:43" s="3" customFormat="1" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>10</v>
@@ -2623,11 +2668,8 @@
       </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>148</v>
+      <c r="B11" s="16">
+        <v>44128</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>123</v>
@@ -2636,43 +2678,104 @@
         <v>124</v>
       </c>
       <c r="E11" s="9">
-        <v>0.97450000000000003</v>
+        <v>0.8619</v>
       </c>
       <c r="F11" s="9">
-        <v>0.91869999999999996</v>
+        <v>0.98929999999999996</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="6">
+        <v>494</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H11" s="6">
+      <c r="J11" s="6">
+        <v>767</v>
+      </c>
+      <c r="K11" s="6">
+        <v>691</v>
+      </c>
+      <c r="L11" s="6">
+        <v>68</v>
+      </c>
+      <c r="M11" s="6">
+        <v>8</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J11" s="6">
-        <v>1584</v>
-      </c>
-      <c r="K11" s="6">
-        <v>1491</v>
-      </c>
-      <c r="L11" s="6">
-        <v>39</v>
-      </c>
-      <c r="M11" s="6">
-        <v>54</v>
-      </c>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="Z11" s="10"/>
-      <c r="AA11" s="10"/>
-      <c r="AB11"/>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="6"/>
-      <c r="AE11" s="6"/>
-      <c r="AF11" s="6"/>
-      <c r="AG11" s="6"/>
-      <c r="AH11" s="6"/>
-      <c r="AI11" s="6"/>
-      <c r="AJ11" s="6"/>
-      <c r="AK11" s="6"/>
+      <c r="O11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="P11" s="9">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>0.95709999999999995</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="S11" s="6">
+        <v>10</v>
+      </c>
+      <c r="T11" s="6">
+        <v>63</v>
+      </c>
+      <c r="U11" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="W11" s="9">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="X11" s="9">
+        <v>0.95979999999999999</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z11" s="10">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="10">
+        <v>67</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG11" s="6">
+        <v>10</v>
+      </c>
+      <c r="AH11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI11" s="6">
+        <v>10</v>
+      </c>
+      <c r="AJ11" s="6">
+        <v>10</v>
+      </c>
+      <c r="AK11" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="AL11" s="6"/>
       <c r="AM11" s="6"/>
       <c r="AN11" s="6"/>
@@ -2685,82 +2788,82 @@
         <v>44128</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E12" s="9">
-        <v>0.8619</v>
+        <v>0.87980000000000003</v>
       </c>
       <c r="F12" s="9">
-        <v>0.98929999999999996</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>39</v>
+        <v>139</v>
       </c>
       <c r="H12" s="6">
-        <v>494</v>
+        <v>650</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="J12" s="6">
-        <v>767</v>
+        <v>2923</v>
       </c>
       <c r="K12" s="6">
-        <v>691</v>
+        <v>2541</v>
       </c>
       <c r="L12" s="6">
-        <v>68</v>
+        <v>320</v>
       </c>
       <c r="M12" s="6">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="P12" s="9">
-        <v>0.76359999999999995</v>
+        <v>0.77990000000000004</v>
       </c>
       <c r="Q12" s="9">
-        <v>0.95709999999999995</v>
+        <v>0.91790000000000005</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="S12" s="6">
         <v>10</v>
       </c>
       <c r="T12" s="6">
-        <v>63</v>
+        <v>138</v>
       </c>
       <c r="U12" s="6" t="s">
-        <v>132</v>
+        <v>72</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="W12" s="9">
-        <v>0.76359999999999995</v>
+        <v>0.77990000000000004</v>
       </c>
       <c r="X12" s="9">
-        <v>0.95979999999999999</v>
+        <v>0.94120000000000004</v>
       </c>
       <c r="Y12" s="6" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="Z12" s="10">
         <v>10</v>
       </c>
       <c r="AA12" s="10">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="AB12" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="AC12" s="6" t="s">
         <v>14</v>
@@ -2798,85 +2901,85 @@
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B13" s="16">
-        <v>44128</v>
+        <v>44135</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E13" s="9">
-        <v>0.87980000000000003</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="F13" s="9">
-        <v>0.98599999999999999</v>
+        <v>0.94340000000000002</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H13" s="6">
-        <v>650</v>
+        <v>17</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="J13" s="6">
-        <v>2923</v>
+        <v>356</v>
       </c>
       <c r="K13" s="6">
-        <v>2541</v>
+        <v>223</v>
       </c>
       <c r="L13" s="6">
-        <v>320</v>
+        <v>112</v>
       </c>
       <c r="M13" s="6">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="P13" s="9">
-        <v>0.77990000000000004</v>
+        <v>0.45079999999999998</v>
       </c>
       <c r="Q13" s="9">
-        <v>0.91790000000000005</v>
+        <v>0.91510000000000002</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="S13" s="6">
         <v>10</v>
       </c>
       <c r="T13" s="6">
-        <v>138</v>
+        <v>3</v>
       </c>
       <c r="U13" s="6" t="s">
-        <v>72</v>
+        <v>152</v>
       </c>
       <c r="V13" s="6" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="W13" s="9">
-        <v>0.77990000000000004</v>
+        <v>0.45079999999999998</v>
       </c>
       <c r="X13" s="9">
-        <v>0.94120000000000004</v>
+        <v>0.91510000000000002</v>
       </c>
       <c r="Y13" s="6" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="Z13" s="10">
         <v>10</v>
       </c>
       <c r="AA13" s="10">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="AB13" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="AC13" s="6" t="s">
         <v>14</v>
@@ -2913,20 +3016,114 @@
       <c r="AQ13" s="6"/>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="10"/>
-      <c r="AB14"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="6"/>
-      <c r="AH14" s="6"/>
-      <c r="AI14" s="6"/>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="6"/>
+      <c r="B14" s="16">
+        <v>44138</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.81540000000000001</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0.98409999999999997</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H14" s="6">
+        <v>511</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="J14" s="6">
+        <v>3630</v>
+      </c>
+      <c r="K14" s="6">
+        <v>3266</v>
+      </c>
+      <c r="L14" s="6">
+        <v>285</v>
+      </c>
+      <c r="M14" s="6">
+        <v>79</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="P14" s="9">
+        <v>0.71540000000000004</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>0.90080000000000005</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="S14" s="6">
+        <v>10</v>
+      </c>
+      <c r="T14" s="6">
+        <v>75</v>
+      </c>
+      <c r="U14" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="W14" s="9">
+        <v>0.71540000000000004</v>
+      </c>
+      <c r="X14" s="9">
+        <v>0.93</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z14" s="10">
+        <v>10</v>
+      </c>
+      <c r="AA14" s="10">
+        <v>81</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG14" s="6">
+        <v>10</v>
+      </c>
+      <c r="AH14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI14" s="6">
+        <v>10</v>
+      </c>
+      <c r="AJ14" s="6">
+        <v>10</v>
+      </c>
+      <c r="AK14" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="AL14" s="6"/>
       <c r="AM14" s="6"/>
       <c r="AN14" s="6"/>
@@ -2978,7 +3175,7 @@
       <c r="AP16" s="6"/>
       <c r="AQ16" s="6"/>
     </row>
-    <row r="17" spans="19:43" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:43" x14ac:dyDescent="0.3">
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="Z17" s="10"/>
@@ -3000,7 +3197,7 @@
       <c r="AP17" s="6"/>
       <c r="AQ17" s="6"/>
     </row>
-    <row r="18" spans="19:43" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:43" x14ac:dyDescent="0.3">
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
       <c r="Z18" s="10"/>
@@ -3022,7 +3219,7 @@
       <c r="AP18" s="6"/>
       <c r="AQ18" s="6"/>
     </row>
-    <row r="19" spans="19:43" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:43" x14ac:dyDescent="0.3">
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
       <c r="Z19" s="10"/>
@@ -3044,7 +3241,7 @@
       <c r="AP19" s="6"/>
       <c r="AQ19" s="6"/>
     </row>
-    <row r="20" spans="19:43" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:43" x14ac:dyDescent="0.3">
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
       <c r="Z20" s="10"/>
@@ -3066,7 +3263,7 @@
       <c r="AP20" s="6"/>
       <c r="AQ20" s="6"/>
     </row>
-    <row r="21" spans="19:43" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:43" x14ac:dyDescent="0.3">
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
       <c r="Z21" s="10"/>
@@ -3088,7 +3285,7 @@
       <c r="AP21" s="6"/>
       <c r="AQ21" s="6"/>
     </row>
-    <row r="22" spans="19:43" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:43" x14ac:dyDescent="0.3">
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
       <c r="Z22" s="10"/>
@@ -3110,7 +3307,7 @@
       <c r="AP22" s="6"/>
       <c r="AQ22" s="6"/>
     </row>
-    <row r="23" spans="19:43" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:43" x14ac:dyDescent="0.3">
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
       <c r="Z23" s="10"/>
@@ -3132,6 +3329,11 @@
       <c r="AP23" s="6"/>
       <c r="AQ23" s="6"/>
     </row>
+    <row r="24" spans="5:43" x14ac:dyDescent="0.3">
+      <c r="E24" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:C2"/>
@@ -3150,18 +3352,17 @@
     <hyperlink ref="C9" r:id="rId6" xr:uid="{ADC87C0F-7720-435C-A768-08162ADFAD58}"/>
     <hyperlink ref="C7" r:id="rId7" xr:uid="{50CB9473-4D34-42DC-A1E2-331AD6C7864F}"/>
     <hyperlink ref="C10" r:id="rId8" xr:uid="{2AD2D1E5-BBEF-4677-89E1-016A7A0FAED2}"/>
-    <hyperlink ref="C11" r:id="rId9" xr:uid="{4F3F9952-CD80-43C4-8E08-6BEDF02F5E83}"/>
-    <hyperlink ref="C12" r:id="rId10" xr:uid="{EB0E65A1-9A5A-4535-8388-CB944B64DA5C}"/>
-    <hyperlink ref="C13" r:id="rId11" xr:uid="{7A637256-9C99-4D41-A244-8C5EE2AFEF9C}"/>
+    <hyperlink ref="C11" r:id="rId9" display="shortid@2.2.16" xr:uid="{B888CDFE-6A23-42E0-8CA1-53F217448B93}"/>
+    <hyperlink ref="C14" r:id="rId10" xr:uid="{E399C88D-FCD1-4571-B019-AEF8F40F42C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
   <tableParts count="5">
+    <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
     <tablePart r:id="rId16"/>
-    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added new information in report, and updated mutode information for both debug version and newer body-parser version
</commit_message>
<xml_diff>
--- a/experiments/AlgoComparisons.xlsx
+++ b/experiments/AlgoComparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\mutode_research\newDD\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233F351C-94A7-4048-AA02-6A705E28265D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1349D752-E61D-4CF5-8B65-F5B20304D1DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2239" yWindow="2239" windowWidth="18850" windowHeight="9844" xr2:uid="{1807BA8C-4E5D-4B92-917C-C9945C819F91}"/>
+    <workbookView xWindow="759" yWindow="759" windowWidth="18851" windowHeight="9845" xr2:uid="{1807BA8C-4E5D-4B92-917C-C9945C819F91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="175">
   <si>
     <t>ddMin</t>
   </si>
@@ -374,18 +376,6 @@
     <t>Mutode Running Time</t>
   </si>
   <si>
-    <t>Mutants Killed2</t>
-  </si>
-  <si>
-    <t>Mutants Generated</t>
-  </si>
-  <si>
-    <t>Mutants Survived</t>
-  </si>
-  <si>
-    <t>Mutants Discarded</t>
-  </si>
-  <si>
     <t>43m 53s</t>
   </si>
   <si>
@@ -536,14 +526,53 @@
     <t>398ms</t>
   </si>
   <si>
-    <t>Note : The mutation scores qouted above are not what the original tool returned, those can be calculated by the killed,survived, discarded mutant given ahead. However this mutation score is computed after we discard a few more mutants, that we not valid for analysis (for example entire test suite failed due to compilation error introduced by a mutation)</t>
+    <t>Orginal  Mutants Discarded</t>
+  </si>
+  <si>
+    <t>Original Mutants Survived</t>
+  </si>
+  <si>
+    <t>Original Mutants Killed</t>
+  </si>
+  <si>
+    <t>Orignal Mutants Generated</t>
+  </si>
+  <si>
+    <t>More Mutants Discarded</t>
+  </si>
+  <si>
+    <t>Updated Killed Mutants</t>
+  </si>
+  <si>
+    <t>Updated Survived Mutant</t>
+  </si>
+  <si>
+    <t>Out of Non discarded Mutants</t>
+  </si>
+  <si>
+    <t>Remaining Killed mutants</t>
+  </si>
+  <si>
+    <t>Remaining survived mutants</t>
+  </si>
+  <si>
+    <t>Calculated as UpdatedKilledMutants / Original Generated Mutants - (Original Mutants Discarded + More Mutants Discarded)</t>
+  </si>
+  <si>
+    <t>Calculated as Original Killed Mutants / Original Generated Mutants - (Original Mutants Discarded)</t>
+  </si>
+  <si>
+    <t>Original Mutation Score</t>
+  </si>
+  <si>
+    <t>Updated Mutation Score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -652,6 +681,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -747,7 +784,7 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -809,6 +846,14 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Accent2" xfId="7" builtinId="33"/>
@@ -821,7 +866,19 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1" xfId="5" xr:uid="{F4E56029-7EE9-453F-ADCF-12C8305BF6E8}"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="53">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1064,80 +1121,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{952538F1-7DF3-4D7D-A8CC-BE4F7FA56AC6}" name="Table8" displayName="Table8" ref="N2:T23" totalsRowShown="0" headerRowDxfId="48" tableBorderDxfId="47" headerRowCellStyle="Explanatory Text">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{952538F1-7DF3-4D7D-A8CC-BE4F7FA56AC6}" name="Table8" displayName="Table8" ref="R2:X23" totalsRowShown="0" headerRowDxfId="52" tableBorderDxfId="51" headerRowCellStyle="Explanatory Text">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{12B54DEA-7254-4D41-BEC3-BEA4C9B5FD2B}" name="AlgorithmRunningTime" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{C041EDEE-7D1D-40B4-A76F-BE7D7A036172}" name="Reduced Subset" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{2D65E345-C673-4CC1-939C-6D0BF18353C1}" name="Mutation Score" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{4CC4BD8C-4EF4-43AB-BAAB-4E7F5B7FD70D}" name="Coverage" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{644740EE-5F30-46BC-A81B-59EA94F094F2}" name="ReducedTestSuiteRunningTime" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{6C008CB6-3003-451B-83F5-7A2E2094A09F}" name="Tolerance" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{D105531A-8670-4AD8-BDF7-70ED045D32AA}" name="ReducedTestSuiteSize" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{12B54DEA-7254-4D41-BEC3-BEA4C9B5FD2B}" name="AlgorithmRunningTime" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{C041EDEE-7D1D-40B4-A76F-BE7D7A036172}" name="Reduced Subset" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{2D65E345-C673-4CC1-939C-6D0BF18353C1}" name="Mutation Score" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{4CC4BD8C-4EF4-43AB-BAAB-4E7F5B7FD70D}" name="Coverage" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{644740EE-5F30-46BC-A81B-59EA94F094F2}" name="ReducedTestSuiteRunningTime" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{6C008CB6-3003-451B-83F5-7A2E2094A09F}" name="Tolerance" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{D105531A-8670-4AD8-BDF7-70ED045D32AA}" name="ReducedTestSuiteSize" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{14F4EC92-7BFE-403F-A3C6-CD427D010934}" name="Table9" displayName="Table9" ref="U2:AA23" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37" headerRowCellStyle="Explanatory Text">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{14F4EC92-7BFE-403F-A3C6-CD427D010934}" name="Table9" displayName="Table9" ref="Y2:AE23" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41" headerRowCellStyle="Explanatory Text">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6C9C0781-48E2-4FB7-8744-C1EDD4F95DCB}" name="AlgorithmRunningTime" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{DA4A4864-0763-4B71-A651-ED4CA4A414F2}" name="Reduced Subset" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{0303DEB1-3A97-457B-8F0B-075435BD2CA4}" name="Mutation Score" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{37441378-B4C1-4801-8946-B5F26FB1A9B8}" name="Coverage" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{5676F7B9-8FF9-49ED-8633-08C2401FF4B2}" name="ReducedTestSuiteRunningTime" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{7E74752D-6DE1-4C73-B537-CFA8D85EDF85}" name="Tolerance" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{2D9D7CF3-D3B4-464C-B1F1-62F1441FBB67}" name="TestSuite Size" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{6C9C0781-48E2-4FB7-8744-C1EDD4F95DCB}" name="AlgorithmRunningTime" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{DA4A4864-0763-4B71-A651-ED4CA4A414F2}" name="Reduced Subset" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{0303DEB1-3A97-457B-8F0B-075435BD2CA4}" name="Mutation Score" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{37441378-B4C1-4801-8946-B5F26FB1A9B8}" name="Coverage" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{5676F7B9-8FF9-49ED-8633-08C2401FF4B2}" name="ReducedTestSuiteRunningTime" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{7E74752D-6DE1-4C73-B537-CFA8D85EDF85}" name="Tolerance" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{2D9D7CF3-D3B4-464C-B1F1-62F1441FBB67}" name="TestSuite Size" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{21AC0CEF-D177-4D66-B441-7618BEEDE8E3}" name="Table10" displayName="Table10" ref="AB2:AK23" totalsRowShown="0" headerRowDxfId="29" tableBorderDxfId="28" headerRowCellStyle="Explanatory Text">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{21AC0CEF-D177-4D66-B441-7618BEEDE8E3}" name="Table10" displayName="Table10" ref="AF2:AO23" totalsRowShown="0" headerRowDxfId="33" tableBorderDxfId="32" headerRowCellStyle="Explanatory Text">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{9B95FA3B-E111-47B3-9FEB-6E34F77C693F}" name="AlgorithmRunningTime"/>
-    <tableColumn id="2" xr3:uid="{CE31A1F2-CCFB-41B9-802E-E4E7D6C22363}" name="Reduced Subset" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{C3588D6B-9C88-46A6-AD70-75921A04F317}" name="Mutation Score" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{640DAF15-6CE5-424F-B23B-0356D0396E43}" name="Coverage" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{72017D7E-EB7B-455E-8490-433A112AD377}" name="ReducedTestSuiteRunningTime" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{2495EE0C-328B-4914-946A-3D5B24547ED9}" name="Starting Tolerance" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{42E4F09C-725B-46FD-8BC3-921A3329D1A6}" name="ToleranceThatFoundASet" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{8E19AD31-C6CB-4914-89F0-9353B6A7CD33}" name="TotalRuns" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{DB462F9A-ABEA-418C-81ED-46797C03550C}" name="ExecutedRuns" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{59135B1B-35D4-4DDB-B9C3-6D510C325029}" name="TestSuite Size" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{CE31A1F2-CCFB-41B9-802E-E4E7D6C22363}" name="Reduced Subset" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{C3588D6B-9C88-46A6-AD70-75921A04F317}" name="Mutation Score" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{640DAF15-6CE5-424F-B23B-0356D0396E43}" name="Coverage" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{72017D7E-EB7B-455E-8490-433A112AD377}" name="ReducedTestSuiteRunningTime" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{2495EE0C-328B-4914-946A-3D5B24547ED9}" name="Starting Tolerance" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{42E4F09C-725B-46FD-8BC3-921A3329D1A6}" name="ToleranceThatFoundASet" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{8E19AD31-C6CB-4914-89F0-9353B6A7CD33}" name="TotalRuns" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{DB462F9A-ABEA-418C-81ED-46797C03550C}" name="ExecutedRuns" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{59135B1B-35D4-4DDB-B9C3-6D510C325029}" name="TestSuite Size" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{750652E7-E767-41D1-9927-FDCE55E1E6D0}" name="Table12" displayName="Table12" ref="D1:M24" totalsRowShown="0" headerRowDxfId="18" headerRowCellStyle="Neutral">
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{15CF07D5-B71B-4A28-8125-12ACDB9CC697}" name="Original Set" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{0D187438-7867-4CF4-BC39-4C5405F1DE55}" name="Mutation Score" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{3699F74C-ECE0-4B26-9682-8D573AD734B8}" name="Coverage" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{CD2ECBD2-6A54-4B63-8B16-769F2F08101F}" name="OriginalTestSuiteRunningTime" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{1D29439A-E95C-4EAB-9C6A-44F1FBC75F33}" name="Orignal TestSuite Size" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{1ED35EFA-8CCC-4F74-B0BA-63D0F2B0C067}" name="Mutode Running Time" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{B31DCAD0-6793-4E02-937E-37FDBF007C2A}" name="Mutants Generated" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{1D18328C-BCA6-4FAC-B58B-4BBF7D4449EA}" name="Mutants Killed2" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{6EED791C-77AD-4042-BF9C-F7480F2D4091}" name="Mutants Survived" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{B04458F3-7CA1-40EA-8E87-222BB12FE8D9}" name="Mutants Discarded" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{750652E7-E767-41D1-9927-FDCE55E1E6D0}" name="Table12" displayName="Table12" ref="D1:Q29" totalsRowShown="0" headerRowDxfId="22" headerRowCellStyle="Neutral">
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{15CF07D5-B71B-4A28-8125-12ACDB9CC697}" name="Original Set" dataDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{8040B8DD-BF4F-4AF5-9E6F-31B248E7BD01}" name="Original Mutation Score" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{0D187438-7867-4CF4-BC39-4C5405F1DE55}" name="Updated Mutation Score" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{3699F74C-ECE0-4B26-9682-8D573AD734B8}" name="Coverage" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{CD2ECBD2-6A54-4B63-8B16-769F2F08101F}" name="OriginalTestSuiteRunningTime" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{1D29439A-E95C-4EAB-9C6A-44F1FBC75F33}" name="Orignal TestSuite Size" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{1ED35EFA-8CCC-4F74-B0BA-63D0F2B0C067}" name="Mutode Running Time" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{B31DCAD0-6793-4E02-937E-37FDBF007C2A}" name="Orignal Mutants Generated" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{1D18328C-BCA6-4FAC-B58B-4BBF7D4449EA}" name="Original Mutants Killed" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{6EED791C-77AD-4042-BF9C-F7480F2D4091}" name="Original Mutants Survived" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{E3E0C4FE-273D-4C62-984B-F580EF6C1842}" name="Orginal  Mutants Discarded" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{6DF9451B-7D78-466A-B72A-F85A75EAEC85}" name="More Mutants Discarded" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{BB220918-6952-4D3F-8B3B-9016EA4A46E0}" name="Updated Killed Mutants" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{B04458F3-7CA1-40EA-8E87-222BB12FE8D9}" name="Updated Survived Mutant" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0109829-D30D-42C3-9E57-90E25F812D9E}" name="Table2" displayName="Table2" ref="AL2:AQ23" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0109829-D30D-42C3-9E57-90E25F812D9E}" name="Table2" displayName="Table2" ref="AP2:AU23" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10" headerRowCellStyle="Accent2">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E4B25968-3AB6-460C-BC4A-98BCD3ED878C}" name="AlgorithmRunningTime" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{3DDDEECD-8312-4190-AA68-6A4E84D065A9}" name="Features to be selected" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{6FD36AEB-1C1B-4058-AE87-EA5A28CA5C75}" name="Reduced Subset" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{F3703558-BD53-4188-AEE9-6233EB063F72}" name="Mutation Score" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{4D7349A3-5B31-4CC5-A72F-4B706196187A}" name="Coverage" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{ED760C3C-7A39-4043-B686-87F211ABDA26}" name="ReducedTestSuiteRunningTime" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E4B25968-3AB6-460C-BC4A-98BCD3ED878C}" name="AlgorithmRunningTime" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{3DDDEECD-8312-4190-AA68-6A4E84D065A9}" name="Features to be selected" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{6FD36AEB-1C1B-4058-AE87-EA5A28CA5C75}" name="Reduced Subset" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{F3703558-BD53-4188-AEE9-6233EB063F72}" name="Mutation Score" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{4D7349A3-5B31-4CC5-A72F-4B706196187A}" name="Coverage" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{ED760C3C-7A39-4043-B686-87F211ABDA26}" name="ReducedTestSuiteRunningTime" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1440,10 +1501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A84B95-A035-4AC9-8702-F9EE4E2D8975}">
-  <dimension ref="A1:AQ24"/>
+  <dimension ref="A1:AU29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1452,45 +1513,47 @@
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" style="6" customWidth="1"/>
     <col min="7" max="7" width="33.44140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="26" style="6" customWidth="1"/>
+    <col min="8" max="8" width="28.88671875" style="6" customWidth="1"/>
     <col min="9" max="9" width="26.44140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="19.5546875" style="6" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="29.109375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" style="6" customWidth="1"/>
-    <col min="14" max="14" width="20.21875" style="6" customWidth="1"/>
-    <col min="15" max="15" width="16.5546875" style="6" customWidth="1"/>
-    <col min="16" max="16" width="10.44140625" style="6" customWidth="1"/>
-    <col min="17" max="17" width="28.77734375" style="6" customWidth="1"/>
-    <col min="18" max="18" width="27" style="6" customWidth="1"/>
-    <col min="19" max="19" width="15.44140625" style="10" customWidth="1"/>
-    <col min="20" max="20" width="22.88671875" customWidth="1"/>
-    <col min="21" max="21" width="19.5546875" style="6" customWidth="1"/>
-    <col min="22" max="22" width="27.44140625" style="6" customWidth="1"/>
-    <col min="23" max="23" width="14.33203125" style="6" customWidth="1"/>
-    <col min="24" max="24" width="27" style="6" customWidth="1"/>
-    <col min="25" max="25" width="22.21875" style="6" customWidth="1"/>
-    <col min="26" max="26" width="18.77734375" style="6" customWidth="1"/>
-    <col min="27" max="27" width="8.88671875" style="6" customWidth="1"/>
-    <col min="28" max="28" width="14.33203125" style="6" customWidth="1"/>
-    <col min="29" max="31" width="8.88671875" customWidth="1"/>
-    <col min="32" max="32" width="15.5546875" customWidth="1"/>
-    <col min="33" max="34" width="24.6640625" customWidth="1"/>
-    <col min="35" max="35" width="22" customWidth="1"/>
-    <col min="36" max="36" width="23.44140625" customWidth="1"/>
-    <col min="37" max="37" width="20.88671875" customWidth="1"/>
-    <col min="38" max="38" width="34.6640625" customWidth="1"/>
+    <col min="10" max="10" width="32.88671875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="25.44140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="26.21875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="29.77734375" style="6" customWidth="1"/>
+    <col min="14" max="15" width="29.109375" style="6" customWidth="1"/>
+    <col min="16" max="16" width="25.44140625" style="6" customWidth="1"/>
+    <col min="17" max="17" width="20.21875" style="6" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" style="6" customWidth="1"/>
+    <col min="19" max="19" width="10.44140625" style="6" customWidth="1"/>
+    <col min="20" max="20" width="28.77734375" style="6" customWidth="1"/>
+    <col min="21" max="21" width="27" style="6" customWidth="1"/>
+    <col min="22" max="22" width="15.44140625" style="10" customWidth="1"/>
+    <col min="23" max="23" width="22.88671875" customWidth="1"/>
+    <col min="24" max="24" width="19.5546875" style="6" customWidth="1"/>
+    <col min="25" max="25" width="27.44140625" style="6" customWidth="1"/>
+    <col min="26" max="26" width="14.33203125" style="6" customWidth="1"/>
+    <col min="27" max="27" width="27" style="6" customWidth="1"/>
+    <col min="28" max="28" width="22.21875" style="6" customWidth="1"/>
+    <col min="29" max="29" width="18.77734375" style="6" customWidth="1"/>
+    <col min="30" max="30" width="8.88671875" style="6" customWidth="1"/>
+    <col min="31" max="31" width="14.33203125" style="6" customWidth="1"/>
+    <col min="32" max="34" width="8.88671875" customWidth="1"/>
+    <col min="35" max="35" width="15.5546875" customWidth="1"/>
+    <col min="36" max="37" width="24.6640625" customWidth="1"/>
+    <col min="38" max="38" width="22" customWidth="1"/>
+    <col min="39" max="39" width="23.44140625" customWidth="1"/>
+    <col min="40" max="40" width="20.88671875" customWidth="1"/>
+    <col min="41" max="41" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="3" customFormat="1" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>144</v>
+    <row r="1" spans="1:47" s="3" customFormat="1" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>10</v>
@@ -1499,76 +1562,94 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>5</v>
+        <v>173</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="12" t="s">
-        <v>112</v>
-      </c>
       <c r="K1" s="12" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="N1" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
       <c r="S1" s="19"/>
       <c r="T1" s="19"/>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
       <c r="Z1" s="20"/>
       <c r="AA1" s="20"/>
-      <c r="AB1" s="21" t="s">
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
       <c r="AG1" s="21"/>
       <c r="AH1" s="21"/>
       <c r="AI1" s="21"/>
       <c r="AJ1" s="21"/>
       <c r="AK1" s="21"/>
-      <c r="AL1" s="22" t="s">
+      <c r="AL1" s="21"/>
+      <c r="AM1" s="21"/>
+      <c r="AN1" s="21"/>
+      <c r="AO1" s="21"/>
+      <c r="AP1" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22"/>
       <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
     </row>
-    <row r="2" spans="1:43" s="1" customFormat="1" ht="20.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" s="1" customFormat="1" ht="20.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>171</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -1576,1571 +1657,1746 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="7"/>
+      <c r="O2" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="P2" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AF2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AE2" s="8" t="s">
+      <c r="AI2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AJ2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AL2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="AI2" s="8" t="s">
+      <c r="AM2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AJ2" s="8" t="s">
+      <c r="AN2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AK2" s="8" t="s">
+      <c r="AO2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AL2" s="13" t="s">
+      <c r="AP2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AQ2" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="AN2" s="14" t="s">
+      <c r="AR2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="AO2" s="14" t="s">
+      <c r="AS2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AP2" s="14" t="s">
+      <c r="AT2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="AQ2" s="14" t="s">
+      <c r="AU2" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="C3" s="25" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="9">
-        <v>0.92769999999999997</v>
-      </c>
-      <c r="F3" s="9">
+      <c r="E3" s="6">
+        <f>ROUND(L3/(K3-N3) * 100,2)</f>
+        <v>92.83</v>
+      </c>
+      <c r="F3" s="6">
+        <f>ROUND((P3/(K3-(O3+N3)))*100,2)</f>
+        <v>92.77</v>
+      </c>
+      <c r="G3" s="9">
         <v>0.92330000000000001</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="6">
         <v>17</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="J3" s="6">
+      <c r="J3" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="K3" s="6">
         <v>2891</v>
       </c>
-      <c r="K3" s="6">
-        <v>2655</v>
-      </c>
       <c r="L3" s="6">
-        <v>208</v>
+        <v>2666</v>
       </c>
       <c r="M3" s="6">
-        <v>28</v>
-      </c>
-      <c r="N3" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="N3" s="6">
+        <v>19</v>
+      </c>
+      <c r="O3" s="6">
+        <v>22</v>
+      </c>
+      <c r="P3" s="6">
+        <v>2644</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>206</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="9">
+      <c r="T3" s="9">
         <v>0.85160000000000002</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="U3" s="9">
         <v>0.71699999999999997</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="6">
-        <v>10</v>
-      </c>
-      <c r="T3" s="6">
+      <c r="W3" s="6">
+        <v>10</v>
+      </c>
+      <c r="X3" s="6">
         <v>2</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="9">
+      <c r="AA3" s="9">
         <v>0.85160000000000002</v>
       </c>
-      <c r="X3" s="9">
+      <c r="AB3" s="9">
         <v>0.71699999999999997</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="10">
-        <v>10</v>
-      </c>
-      <c r="AA3" s="10">
+      <c r="AD3" s="10">
+        <v>10</v>
+      </c>
+      <c r="AE3" s="10">
         <v>2</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AF3" t="s">
         <v>47</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AG3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AD3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG3" s="6">
-        <v>10</v>
-      </c>
       <c r="AH3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AI3" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ3" s="6">
-        <v>10</v>
-      </c>
-      <c r="AK3" s="6" t="s">
-        <v>15</v>
+      <c r="AI3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK3" s="6">
+        <v>10</v>
       </c>
       <c r="AL3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM3" s="6">
+        <v>10</v>
+      </c>
+      <c r="AN3" s="6">
+        <v>10</v>
+      </c>
+      <c r="AO3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AM3" s="6">
+      <c r="AQ3" s="6">
         <v>8</v>
       </c>
-      <c r="AN3" s="6" t="s">
+      <c r="AR3" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="AO3" s="9">
+      <c r="AS3" s="9">
         <v>0.92559999999999998</v>
       </c>
-      <c r="AP3" s="9">
+      <c r="AT3" s="9">
         <v>0.91410000000000002</v>
       </c>
-      <c r="AQ3" s="6" t="s">
+      <c r="AU3" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="C4" s="25" t="s">
         <v>55</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
+        <f>ROUND(L4/(K4-N4) * 100,2)</f>
+        <v>8.33</v>
+      </c>
+      <c r="F4" s="6">
+        <f>ROUND((P4/(K4-(O4+N4)))*100,2)</f>
+        <v>3.68</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.68669999999999998</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="6">
+        <v>4</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1300</v>
+      </c>
+      <c r="L4" s="6">
+        <v>107</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1177</v>
+      </c>
+      <c r="N4" s="6">
+        <v>16</v>
+      </c>
+      <c r="O4" s="6">
+        <v>62</v>
+      </c>
+      <c r="P4" s="6">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>1177</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="6">
+        <v>3</v>
+      </c>
+      <c r="T4" s="9">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="F4" s="9">
-        <v>0.68669999999999998</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="6">
-        <v>4</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="J4" s="6">
-        <v>1300</v>
-      </c>
-      <c r="K4" s="6">
-        <v>106</v>
-      </c>
-      <c r="L4" s="6">
-        <v>1189</v>
-      </c>
-      <c r="M4" s="6">
-        <v>5</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" s="6">
+      <c r="U4" s="9">
+        <v>0.43330000000000002</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="W4" s="6">
+        <v>10</v>
+      </c>
+      <c r="X4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z4" s="6">
         <v>3</v>
       </c>
-      <c r="P4" s="9">
+      <c r="AA4" s="9">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="Q4" s="9">
-        <v>0.43330000000000002</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="6">
-        <v>10</v>
-      </c>
-      <c r="T4" s="6">
+      <c r="AB4" s="9">
+        <v>0.69610000000000005</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD4" s="10">
         <v>1</v>
       </c>
-      <c r="U4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="V4" s="6">
-        <v>3</v>
-      </c>
-      <c r="W4" s="9">
-        <v>3.6799999999999999E-2</v>
-      </c>
-      <c r="X4" s="9">
-        <v>0.69610000000000005</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z4" s="10">
+      <c r="AE4" s="10">
         <v>1</v>
       </c>
-      <c r="AA4" s="10">
-        <v>1</v>
-      </c>
-      <c r="AB4" t="s">
+      <c r="AF4" t="s">
         <v>48</v>
       </c>
-      <c r="AC4" s="6">
+      <c r="AG4" s="6">
         <v>0</v>
       </c>
-      <c r="AD4" s="11">
+      <c r="AH4" s="11">
         <v>0</v>
       </c>
-      <c r="AE4" s="9">
+      <c r="AI4" s="9">
         <v>0.48070000000000002</v>
       </c>
-      <c r="AF4" s="6" t="s">
+      <c r="AJ4" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="AG4" s="6">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="6">
-        <v>3.68</v>
-      </c>
-      <c r="AI4" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ4" s="6">
-        <v>2</v>
       </c>
       <c r="AK4" s="6">
         <v>1</v>
       </c>
-      <c r="AL4" s="6" t="s">
+      <c r="AL4" s="6">
+        <v>3.68</v>
+      </c>
+      <c r="AM4" s="6">
+        <v>10</v>
+      </c>
+      <c r="AN4" s="6">
+        <v>2</v>
+      </c>
+      <c r="AO4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AP4" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="AM4" s="6">
+      <c r="AQ4" s="6">
         <v>2</v>
       </c>
-      <c r="AN4" s="6" t="s">
+      <c r="AR4" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="AO4" s="9">
+      <c r="AS4" s="9">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="AP4" s="11">
+      <c r="AT4" s="11">
         <v>0.68</v>
       </c>
-      <c r="AQ4" s="11" t="s">
+      <c r="AU4" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="C5" s="25" t="s">
         <v>56</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="9">
-        <v>0.74409999999999998</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="E5" s="6">
+        <f>ROUND(L5/(K5-N5) * 100,2)</f>
+        <v>89.09</v>
+      </c>
+      <c r="F5" s="6">
+        <f>ROUND((P5/(K5-(O5+N5)))*100,2)</f>
+        <v>74.41</v>
+      </c>
+      <c r="G5" s="9">
         <v>0.997</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <v>218</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="J5" s="6">
+      <c r="J5" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="K5" s="6">
         <v>976</v>
       </c>
-      <c r="K5" s="6">
-        <v>766</v>
-      </c>
       <c r="L5" s="6">
-        <v>175</v>
+        <v>792</v>
       </c>
       <c r="M5" s="6">
-        <v>35</v>
-      </c>
-      <c r="N5" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="N5" s="6">
+        <v>87</v>
+      </c>
+      <c r="O5" s="6">
+        <v>170</v>
+      </c>
+      <c r="P5" s="6">
+        <v>535</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>184</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="9">
+      <c r="T5" s="9">
         <v>0.64529999999999998</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="U5" s="9">
         <v>0.88549999999999995</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="V5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="S5" s="6">
-        <v>10</v>
-      </c>
-      <c r="T5" s="6">
+      <c r="W5" s="6">
+        <v>10</v>
+      </c>
+      <c r="X5" s="6">
         <v>42</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="Y5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="Z5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="W5" s="9">
+      <c r="AA5" s="9">
         <v>0.64529999999999998</v>
       </c>
-      <c r="X5" s="9">
+      <c r="AB5" s="9">
         <v>0.89159999999999995</v>
       </c>
-      <c r="Y5" s="6" t="s">
+      <c r="AC5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Z5" s="10">
-        <v>10</v>
-      </c>
-      <c r="AA5" s="10">
+      <c r="AD5" s="10">
+        <v>10</v>
+      </c>
+      <c r="AE5" s="10">
         <v>40</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AF5" t="s">
         <v>49</v>
       </c>
-      <c r="AC5" s="6" t="s">
+      <c r="AG5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AD5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG5" s="6">
-        <v>10</v>
-      </c>
       <c r="AH5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AI5" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ5" s="6">
-        <v>10</v>
-      </c>
-      <c r="AK5" s="6" t="s">
-        <v>15</v>
+      <c r="AI5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK5" s="6">
+        <v>10</v>
       </c>
       <c r="AL5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM5" s="6">
+        <v>10</v>
+      </c>
+      <c r="AN5" s="6">
+        <v>10</v>
+      </c>
+      <c r="AO5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP5" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="AM5" s="6">
+      <c r="AQ5" s="6">
         <v>109</v>
       </c>
-      <c r="AN5" s="6" t="s">
+      <c r="AR5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="AO5" s="9">
+      <c r="AS5" s="9">
         <v>0.47149999999999997</v>
       </c>
-      <c r="AP5" s="9">
+      <c r="AT5" s="9">
         <v>0.86729999999999996</v>
       </c>
-      <c r="AQ5" s="6" t="s">
+      <c r="AU5" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="C6" s="25" t="s">
         <v>57</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="9">
-        <v>0.73219999999999996</v>
-      </c>
-      <c r="F6" s="9">
+      <c r="E6" s="6">
+        <f>ROUND(L6/(K6-N6) * 100,2)</f>
+        <v>77.209999999999994</v>
+      </c>
+      <c r="F6" s="6">
+        <f>ROUND((P6/(K6-(O6+N6)))*100,2)</f>
+        <v>73.25</v>
+      </c>
+      <c r="G6" s="9">
         <v>0.98629999999999995</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <v>858</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="J6" s="6">
+      <c r="J6" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" s="6">
         <v>3900</v>
       </c>
-      <c r="K6" s="6">
-        <v>2900</v>
-      </c>
       <c r="L6" s="6">
-        <v>607</v>
+        <v>2483</v>
       </c>
       <c r="M6" s="6">
-        <v>393</v>
-      </c>
-      <c r="N6" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="N6" s="6">
+        <v>684</v>
+      </c>
+      <c r="O6" s="6">
+        <v>480</v>
+      </c>
+      <c r="P6" s="6">
+        <v>2004</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>733</v>
+      </c>
+      <c r="R6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="S6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="9">
+      <c r="T6" s="9">
         <v>0.63239999999999996</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="U6" s="9">
         <v>0.82330000000000003</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="V6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="S6" s="6">
-        <v>10</v>
-      </c>
-      <c r="T6" s="6">
+      <c r="W6" s="6">
+        <v>10</v>
+      </c>
+      <c r="X6" s="6">
         <v>156</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="Y6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="V6" s="9" t="s">
+      <c r="Z6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="W6" s="9">
+      <c r="AA6" s="9">
         <v>0.63239999999999996</v>
       </c>
-      <c r="X6" s="9">
+      <c r="AB6" s="9">
         <v>0.85670000000000002</v>
       </c>
-      <c r="Y6" s="6" t="s">
+      <c r="AC6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Z6" s="10">
-        <v>10</v>
-      </c>
-      <c r="AA6" s="10">
+      <c r="AD6" s="10">
+        <v>10</v>
+      </c>
+      <c r="AE6" s="10">
         <v>144</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AF6" t="s">
         <v>50</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AG6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AD6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG6" s="6">
-        <v>10</v>
-      </c>
       <c r="AH6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AI6" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ6" s="6">
-        <v>10</v>
-      </c>
-      <c r="AK6" s="6" t="s">
-        <v>15</v>
+      <c r="AI6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK6" s="6">
+        <v>10</v>
       </c>
       <c r="AL6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM6" s="6">
+        <v>10</v>
+      </c>
+      <c r="AN6" s="6">
+        <v>10</v>
+      </c>
+      <c r="AO6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP6" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="AM6" s="6">
+      <c r="AQ6" s="6">
         <v>200</v>
       </c>
-      <c r="AN6" s="6" t="s">
+      <c r="AR6" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="AO6" s="9">
+      <c r="AS6" s="9">
         <v>0.29409999999999997</v>
       </c>
-      <c r="AP6" s="9">
+      <c r="AT6" s="9">
         <v>0.71609999999999996</v>
       </c>
-      <c r="AQ6" s="6" t="s">
+      <c r="AU6" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="C7" s="25" t="s">
         <v>74</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="6">
+        <f>ROUND(L7/(K7-N7) * 100,2)</f>
+        <v>7.14</v>
+      </c>
+      <c r="F7" s="6">
+        <f>ROUND((P7/(K7-(O7+N7)))*100,2)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="9">
+      <c r="G7" s="9">
         <v>0.81159999999999999</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I7" s="6">
         <v>8</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="J7" s="6">
+      <c r="J7" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" s="6">
         <v>70</v>
       </c>
-      <c r="K7" s="6">
+      <c r="L7" s="6">
         <v>5</v>
       </c>
-      <c r="L7" s="6">
+      <c r="M7" s="6">
         <v>65</v>
       </c>
-      <c r="M7" s="6">
+      <c r="N7" s="6">
         <v>0</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="O7" s="6">
+        <v>5</v>
+      </c>
+      <c r="P7" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>65</v>
+      </c>
+      <c r="R7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="6">
+      <c r="S7" s="6">
         <v>7</v>
       </c>
-      <c r="P7" s="11">
+      <c r="T7" s="11">
         <v>0</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="U7" s="9">
         <v>0.79710000000000003</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="V7" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="S7" s="6">
-        <v>10</v>
-      </c>
-      <c r="T7" s="6">
+      <c r="W7" s="6">
+        <v>10</v>
+      </c>
+      <c r="X7" s="6">
         <v>1</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="Y7" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="V7" s="6" t="s">
+      <c r="Z7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="W7" s="11">
+      <c r="AA7" s="11">
         <v>0</v>
       </c>
-      <c r="X7" s="11">
+      <c r="AB7" s="11">
         <v>0</v>
       </c>
-      <c r="Y7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z7" s="10">
-        <v>10</v>
-      </c>
-      <c r="AA7" s="10">
+      <c r="AC7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD7" s="10">
+        <v>10</v>
+      </c>
+      <c r="AE7" s="10">
         <v>0</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AF7" t="s">
         <v>80</v>
       </c>
-      <c r="AC7" s="6" t="s">
+      <c r="AG7" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="AD7" s="11">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="9">
-        <v>0.81159999999999999</v>
-      </c>
-      <c r="AF7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG7" s="6">
-        <v>10</v>
       </c>
       <c r="AH7" s="11">
         <v>0</v>
       </c>
-      <c r="AI7" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ7" s="6">
+      <c r="AI7" s="9">
+        <v>0.81159999999999999</v>
+      </c>
+      <c r="AJ7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK7" s="6">
+        <v>10</v>
+      </c>
+      <c r="AL7" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="6">
+        <v>10</v>
+      </c>
+      <c r="AN7" s="6">
         <v>1</v>
       </c>
-      <c r="AK7" s="6">
+      <c r="AO7" s="6">
         <v>7</v>
       </c>
-      <c r="AL7" s="6" t="s">
+      <c r="AP7" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="AM7" s="6">
+      <c r="AQ7" s="6">
         <v>4</v>
       </c>
-      <c r="AN7" s="6" t="s">
+      <c r="AR7" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="AO7" s="11">
+      <c r="AS7" s="11">
         <v>0</v>
       </c>
-      <c r="AP7" s="9">
+      <c r="AT7" s="9">
         <v>0.57450000000000001</v>
       </c>
-      <c r="AQ7" s="6" t="s">
+      <c r="AU7" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="C8" s="25" t="s">
         <v>58</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="9">
-        <v>5.8799999999999998E-2</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="E8" s="6">
+        <f>ROUND(L8/(K8-N8) * 100,2)</f>
+        <v>11.59</v>
+      </c>
+      <c r="F8" s="6">
+        <f>ROUND((P8/(K8-(O8+N8)))*100,2)</f>
+        <v>5.16</v>
+      </c>
+      <c r="G8" s="9">
         <v>0.61180000000000001</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="6">
+      <c r="I8" s="6">
         <v>3</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="J8" s="6">
+      <c r="J8" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K8" s="6">
         <v>814</v>
       </c>
-      <c r="K8" s="6">
+      <c r="L8" s="6">
         <v>94</v>
       </c>
-      <c r="L8" s="6">
+      <c r="M8" s="6">
         <v>717</v>
       </c>
-      <c r="M8" s="6">
+      <c r="N8" s="6">
         <v>3</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="O8" s="6">
+        <v>55</v>
+      </c>
+      <c r="P8" s="6">
+        <v>39</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>717</v>
+      </c>
+      <c r="R8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="O8" s="6">
+      <c r="S8" s="6">
         <v>2</v>
       </c>
-      <c r="P8" s="9">
-        <v>5.8799999999999998E-2</v>
-      </c>
-      <c r="Q8" s="9">
+      <c r="T8" s="9">
+        <v>5.16E-2</v>
+      </c>
+      <c r="U8" s="9">
         <v>0.60529999999999995</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="V8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="S8" s="6">
-        <v>10</v>
-      </c>
-      <c r="T8" s="6">
+      <c r="W8" s="6">
+        <v>10</v>
+      </c>
+      <c r="X8" s="6">
         <v>1</v>
       </c>
-      <c r="U8" s="6" t="s">
+      <c r="Y8" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="V8" s="6">
+      <c r="Z8" s="6">
         <v>2</v>
       </c>
-      <c r="W8" s="9">
-        <v>5.8799999999999998E-2</v>
-      </c>
-      <c r="X8" s="9">
+      <c r="AA8" s="9">
+        <v>5.16E-2</v>
+      </c>
+      <c r="AB8" s="9">
         <v>0.60529999999999995</v>
       </c>
-      <c r="Y8" s="6" t="s">
+      <c r="AC8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="Z8" s="10">
+      <c r="AD8" s="10">
         <v>1</v>
       </c>
-      <c r="AA8" s="10">
+      <c r="AE8" s="10">
         <v>1</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AF8" t="s">
         <v>63</v>
       </c>
-      <c r="AC8" s="6" t="s">
+      <c r="AG8" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AD8" s="11">
+      <c r="AH8" s="11">
         <v>0</v>
       </c>
-      <c r="AE8" s="11">
+      <c r="AI8" s="11">
         <v>0</v>
       </c>
-      <c r="AF8" s="6" t="s">
+      <c r="AJ8" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AG8" s="6">
+      <c r="AK8" s="6">
         <v>1</v>
       </c>
-      <c r="AH8" s="6">
-        <v>5.88</v>
-      </c>
-      <c r="AI8" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ8" s="6">
-        <v>2</v>
-      </c>
-      <c r="AK8" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="6" t="s">
-        <v>78</v>
+      <c r="AL8" s="9">
+        <v>5.16E-2</v>
       </c>
       <c r="AM8" s="6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AN8" s="6">
         <v>2</v>
       </c>
-      <c r="AO8" s="9">
-        <v>5.8799999999999998E-2</v>
-      </c>
-      <c r="AP8" s="9">
+      <c r="AO8" s="6">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ8" s="6">
+        <v>1</v>
+      </c>
+      <c r="AR8" s="6">
+        <v>2</v>
+      </c>
+      <c r="AS8" s="9">
+        <v>5.16E-2</v>
+      </c>
+      <c r="AT8" s="9">
         <v>0.60529999999999995</v>
       </c>
-      <c r="AQ8" s="6" t="s">
+      <c r="AU8" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="C9" s="25" t="s">
         <v>66</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="9">
-        <v>0.77380000000000004</v>
-      </c>
-      <c r="F9" s="11">
+      <c r="E9" s="6">
+        <f>ROUND(L9/(K9-N9) * 100,2)</f>
+        <v>81.7</v>
+      </c>
+      <c r="F9" s="6">
+        <f>ROUND((P9/(K9-(O9+N9)))*100,2)</f>
+        <v>77.38</v>
+      </c>
+      <c r="G9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="6">
+      <c r="I9" s="6">
         <v>204</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J9" s="6">
+      <c r="J9" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K9" s="6">
         <v>885</v>
       </c>
-      <c r="K9" s="6">
+      <c r="L9" s="6">
         <v>701</v>
       </c>
-      <c r="L9" s="6">
+      <c r="M9" s="6">
         <v>157</v>
       </c>
-      <c r="M9" s="6">
+      <c r="N9" s="6">
         <v>27</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="O9" s="6">
+        <v>164</v>
+      </c>
+      <c r="P9" s="6">
+        <v>537</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>157</v>
+      </c>
+      <c r="R9" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="S9" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="P9" s="9">
+      <c r="T9" s="9">
         <v>0.6744</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="U9" s="9">
         <v>0.89339999999999997</v>
       </c>
-      <c r="R9" s="6" t="s">
+      <c r="V9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="S9" s="6">
-        <v>10</v>
-      </c>
-      <c r="T9" s="6">
+      <c r="W9" s="6">
+        <v>10</v>
+      </c>
+      <c r="X9" s="6">
         <v>42</v>
       </c>
-      <c r="U9" s="6" t="s">
+      <c r="Y9" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="V9" s="6" t="s">
+      <c r="Z9" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="W9" s="9">
+      <c r="AA9" s="9">
         <v>0.6744</v>
       </c>
-      <c r="X9" s="9">
+      <c r="AB9" s="9">
         <v>0.89659999999999995</v>
       </c>
-      <c r="Y9" s="6" t="s">
+      <c r="AC9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="Z9" s="10">
-        <v>10</v>
-      </c>
-      <c r="AA9" s="10">
+      <c r="AD9" s="10">
+        <v>10</v>
+      </c>
+      <c r="AE9" s="10">
         <v>35</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AF9" t="s">
         <v>73</v>
       </c>
-      <c r="AC9" s="6" t="s">
+      <c r="AG9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AD9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG9" s="6">
-        <v>10</v>
-      </c>
       <c r="AH9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AI9" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ9" s="6">
-        <v>10</v>
-      </c>
-      <c r="AK9" s="6" t="s">
-        <v>15</v>
+      <c r="AI9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK9" s="6">
+        <v>10</v>
       </c>
       <c r="AL9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM9" s="6">
+        <v>10</v>
+      </c>
+      <c r="AN9" s="6">
+        <v>10</v>
+      </c>
+      <c r="AO9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP9" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="AM9" s="6">
+      <c r="AQ9" s="6">
         <v>102</v>
       </c>
-      <c r="AN9" s="6" t="s">
+      <c r="AR9" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="AO9" s="9">
+      <c r="AS9" s="9">
         <v>0.47120000000000001</v>
       </c>
-      <c r="AP9" s="9">
+      <c r="AT9" s="9">
         <v>0.879</v>
       </c>
-      <c r="AQ9" s="6" t="s">
+      <c r="AU9" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="C10" s="25" t="s">
         <v>83</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="9">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="F10" s="9">
+      <c r="E10" s="6">
+        <f>ROUND(L10/(K10-N10) * 100,2)</f>
+        <v>79.540000000000006</v>
+      </c>
+      <c r="F10" s="6">
+        <f>ROUND((P10/(K10-(O10+N10)))*100,2)</f>
+        <v>76.19</v>
+      </c>
+      <c r="G10" s="9">
         <v>0.98660000000000003</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H10" s="6">
+      <c r="I10" s="6">
         <v>833</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="J10" s="6">
+      <c r="J10" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K10" s="6">
         <v>3788</v>
       </c>
-      <c r="K10" s="6">
+      <c r="L10" s="6">
         <v>2713</v>
       </c>
-      <c r="L10" s="6">
+      <c r="M10" s="6">
         <v>698</v>
       </c>
-      <c r="M10" s="6">
+      <c r="N10" s="6">
         <v>377</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="O10" s="6">
+        <v>480</v>
+      </c>
+      <c r="P10" s="6">
+        <v>2233</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>698</v>
+      </c>
+      <c r="R10" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="S10" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="P10" s="9">
+      <c r="T10" s="9">
         <v>0.66190000000000004</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="U10" s="9">
         <v>0.81289999999999996</v>
       </c>
-      <c r="R10" s="6" t="s">
+      <c r="V10" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="S10" s="6">
-        <v>10</v>
-      </c>
-      <c r="T10" s="6">
+      <c r="W10" s="6">
+        <v>10</v>
+      </c>
+      <c r="X10" s="6">
         <v>148</v>
       </c>
-      <c r="U10" s="6" t="s">
+      <c r="Y10" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="V10" s="6" t="s">
+      <c r="Z10" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="W10" s="9">
+      <c r="AA10" s="9">
         <v>0.66190000000000004</v>
       </c>
-      <c r="X10" s="9">
+      <c r="AB10" s="9">
         <v>0.84930000000000005</v>
       </c>
-      <c r="Y10" s="6" t="s">
+      <c r="AC10" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="Z10" s="10">
-        <v>10</v>
-      </c>
-      <c r="AA10" s="10">
+      <c r="AD10" s="10">
+        <v>10</v>
+      </c>
+      <c r="AE10" s="10">
         <v>129</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AF10" t="s">
         <v>90</v>
       </c>
-      <c r="AC10" s="6" t="s">
+      <c r="AG10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AD10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG10" s="6">
-        <v>10</v>
-      </c>
       <c r="AH10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AI10" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ10" s="6">
-        <v>10</v>
-      </c>
-      <c r="AK10" s="6" t="s">
-        <v>15</v>
+      <c r="AI10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK10" s="6">
+        <v>10</v>
       </c>
       <c r="AL10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM10" s="6">
+        <v>10</v>
+      </c>
+      <c r="AN10" s="6">
+        <v>10</v>
+      </c>
+      <c r="AO10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP10" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="AM10" s="6">
+      <c r="AQ10" s="6">
         <v>200</v>
       </c>
-      <c r="AN10" s="6" t="s">
+      <c r="AR10" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AO10" s="9">
+      <c r="AS10" s="9">
         <v>0.35859999999999997</v>
       </c>
-      <c r="AP10" s="9">
+      <c r="AT10" s="9">
         <v>0.70920000000000005</v>
       </c>
-      <c r="AQ10" s="6" t="s">
+      <c r="AU10" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B11" s="16">
         <v>44128</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="6">
+        <f>ROUND(L11/(K11-N11) * 100,2)</f>
+        <v>91.04</v>
+      </c>
+      <c r="F11" s="6">
+        <f>ROUND((P11/(K11-(O11+N11)))*100,2)</f>
+        <v>86.19</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0.98929999999999996</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="6">
+        <v>494</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" s="6">
+        <v>767</v>
+      </c>
+      <c r="L11" s="6">
+        <v>691</v>
+      </c>
+      <c r="M11" s="6">
+        <v>68</v>
+      </c>
+      <c r="N11" s="6">
+        <v>8</v>
+      </c>
+      <c r="O11" s="6">
+        <v>281</v>
+      </c>
+      <c r="P11" s="6">
+        <v>412</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>66</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="S11" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="T11" s="9">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="U11" s="9">
+        <v>0.95709999999999995</v>
+      </c>
+      <c r="V11" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E11" s="9">
-        <v>0.8619</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0.98929999999999996</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="6">
-        <v>494</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="W11" s="6">
+        <v>10</v>
+      </c>
+      <c r="X11" s="6">
+        <v>63</v>
+      </c>
+      <c r="Y11" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="6">
-        <v>767</v>
-      </c>
-      <c r="K11" s="6">
-        <v>691</v>
-      </c>
-      <c r="L11" s="6">
-        <v>68</v>
-      </c>
-      <c r="M11" s="6">
-        <v>8</v>
-      </c>
-      <c r="N11" s="6" t="s">
+      <c r="Z11" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="AA11" s="9">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="AB11" s="9">
+        <v>0.95979999999999999</v>
+      </c>
+      <c r="AC11" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="P11" s="9">
-        <v>0.76359999999999995</v>
-      </c>
-      <c r="Q11" s="9">
-        <v>0.95709999999999995</v>
-      </c>
-      <c r="R11" s="6" t="s">
+      <c r="AD11" s="10">
+        <v>10</v>
+      </c>
+      <c r="AE11" s="10">
+        <v>67</v>
+      </c>
+      <c r="AF11" t="s">
         <v>128</v>
       </c>
-      <c r="S11" s="6">
-        <v>10</v>
-      </c>
-      <c r="T11" s="6">
-        <v>63</v>
-      </c>
-      <c r="U11" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="V11" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="W11" s="9">
-        <v>0.76359999999999995</v>
-      </c>
-      <c r="X11" s="9">
-        <v>0.95979999999999999</v>
-      </c>
-      <c r="Y11" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="Z11" s="10">
-        <v>10</v>
-      </c>
-      <c r="AA11" s="10">
-        <v>67</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC11" s="6" t="s">
+      <c r="AG11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AD11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG11" s="6">
-        <v>10</v>
-      </c>
       <c r="AH11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AI11" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ11" s="6">
-        <v>10</v>
-      </c>
-      <c r="AK11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL11" s="6"/>
-      <c r="AM11" s="6"/>
-      <c r="AN11" s="6"/>
-      <c r="AO11" s="6"/>
+      <c r="AI11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK11" s="6">
+        <v>10</v>
+      </c>
+      <c r="AL11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM11" s="6">
+        <v>10</v>
+      </c>
+      <c r="AN11" s="6">
+        <v>10</v>
+      </c>
+      <c r="AO11" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="AP11" s="6"/>
       <c r="AQ11" s="6"/>
+      <c r="AR11" s="6"/>
+      <c r="AS11" s="6"/>
+      <c r="AT11" s="6"/>
+      <c r="AU11" s="6"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B12" s="16">
         <v>44128</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="6">
+        <f>ROUND(L12/(K12-N12) * 100,2)</f>
+        <v>88.82</v>
+      </c>
+      <c r="F12" s="6">
+        <f>ROUND((P12/(K12-(O12+N12)))*100,2)</f>
+        <v>87.98</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="I12" s="6">
+        <v>650</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="K12" s="6">
+        <v>2923</v>
+      </c>
+      <c r="L12" s="6">
+        <v>2541</v>
+      </c>
+      <c r="M12" s="6">
+        <v>320</v>
+      </c>
+      <c r="N12" s="6">
+        <v>62</v>
+      </c>
+      <c r="O12" s="6">
+        <v>198</v>
+      </c>
+      <c r="P12" s="6">
+        <v>2343</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>320</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="S12" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="T12" s="9">
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="U12" s="9">
+        <v>0.91790000000000005</v>
+      </c>
+      <c r="V12" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="E12" s="9">
-        <v>0.87980000000000003</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="H12" s="6">
-        <v>650</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="J12" s="6">
-        <v>2923</v>
-      </c>
-      <c r="K12" s="6">
-        <v>2541</v>
-      </c>
-      <c r="L12" s="6">
-        <v>320</v>
-      </c>
-      <c r="M12" s="6">
-        <v>62</v>
-      </c>
-      <c r="N12" s="6" t="s">
+      <c r="W12" s="6">
+        <v>10</v>
+      </c>
+      <c r="X12" s="6">
+        <v>138</v>
+      </c>
+      <c r="Y12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z12" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="AA12" s="9">
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="AB12" s="9">
+        <v>0.94120000000000004</v>
+      </c>
+      <c r="AC12" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="P12" s="9">
-        <v>0.77990000000000004</v>
-      </c>
-      <c r="Q12" s="9">
-        <v>0.91790000000000005</v>
-      </c>
-      <c r="R12" s="6" t="s">
+      <c r="AD12" s="10">
+        <v>10</v>
+      </c>
+      <c r="AE12" s="10">
+        <v>141</v>
+      </c>
+      <c r="AF12" t="s">
         <v>138</v>
       </c>
-      <c r="S12" s="6">
-        <v>10</v>
-      </c>
-      <c r="T12" s="6">
-        <v>138</v>
-      </c>
-      <c r="U12" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="V12" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="W12" s="9">
-        <v>0.77990000000000004</v>
-      </c>
-      <c r="X12" s="9">
-        <v>0.94120000000000004</v>
-      </c>
-      <c r="Y12" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z12" s="10">
-        <v>10</v>
-      </c>
-      <c r="AA12" s="10">
-        <v>141</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>142</v>
-      </c>
-      <c r="AC12" s="6" t="s">
+      <c r="AG12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AD12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG12" s="6">
-        <v>10</v>
-      </c>
       <c r="AH12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AI12" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ12" s="6">
-        <v>10</v>
-      </c>
-      <c r="AK12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL12" s="6"/>
-      <c r="AM12" s="6"/>
-      <c r="AN12" s="6"/>
-      <c r="AO12" s="6"/>
+      <c r="AI12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK12" s="6">
+        <v>10</v>
+      </c>
+      <c r="AL12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM12" s="6">
+        <v>10</v>
+      </c>
+      <c r="AN12" s="6">
+        <v>10</v>
+      </c>
+      <c r="AO12" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="AP12" s="6"/>
       <c r="AQ12" s="6"/>
+      <c r="AR12" s="6"/>
+      <c r="AS12" s="6"/>
+      <c r="AT12" s="6"/>
+      <c r="AU12" s="6"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B13" s="16">
         <v>44135</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="6">
+        <f>ROUND(L13/(K13-N13) * 100,2)</f>
+        <v>66.569999999999993</v>
+      </c>
+      <c r="F13" s="6">
+        <f>ROUND((P13/(K13-(O13+N13)))*100,2)</f>
+        <v>54.1</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.94340000000000002</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="I13" s="6">
+        <v>17</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K13" s="6">
+        <v>356</v>
+      </c>
+      <c r="L13" s="6">
+        <v>223</v>
+      </c>
+      <c r="M13" s="6">
+        <v>112</v>
+      </c>
+      <c r="N13" s="6">
+        <v>21</v>
+      </c>
+      <c r="O13" s="6">
+        <v>91</v>
+      </c>
+      <c r="P13" s="6">
+        <v>132</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>112</v>
+      </c>
+      <c r="R13" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="S13" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="T13" s="9">
+        <v>0.45079999999999998</v>
+      </c>
+      <c r="U13" s="9">
+        <v>0.91510000000000002</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="W13" s="6">
+        <v>10</v>
+      </c>
+      <c r="X13" s="6">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="9">
-        <v>0.54100000000000004</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0.94340000000000002</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H13" s="6">
-        <v>17</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="J13" s="6">
-        <v>356</v>
-      </c>
-      <c r="K13" s="6">
-        <v>223</v>
-      </c>
-      <c r="L13" s="6">
-        <v>112</v>
-      </c>
-      <c r="M13" s="6">
-        <v>21</v>
-      </c>
-      <c r="N13" s="6" t="s">
+      <c r="Z13" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="O13" s="6" t="s">
+      <c r="AA13" s="9">
+        <v>0.45079999999999998</v>
+      </c>
+      <c r="AB13" s="9">
+        <v>0.91510000000000002</v>
+      </c>
+      <c r="AC13" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="P13" s="9">
-        <v>0.45079999999999998</v>
-      </c>
-      <c r="Q13" s="9">
-        <v>0.91510000000000002</v>
-      </c>
-      <c r="R13" s="6" t="s">
+      <c r="AD13" s="10">
+        <v>10</v>
+      </c>
+      <c r="AE13" s="10">
+        <v>3</v>
+      </c>
+      <c r="AF13" t="s">
         <v>151</v>
       </c>
-      <c r="S13" s="6">
-        <v>10</v>
-      </c>
-      <c r="T13" s="6">
-        <v>3</v>
-      </c>
-      <c r="U13" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="V13" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="W13" s="9">
-        <v>0.45079999999999998</v>
-      </c>
-      <c r="X13" s="9">
-        <v>0.91510000000000002</v>
-      </c>
-      <c r="Y13" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z13" s="10">
-        <v>10</v>
-      </c>
-      <c r="AA13" s="10">
-        <v>3</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>155</v>
-      </c>
-      <c r="AC13" s="6" t="s">
+      <c r="AG13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AD13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG13" s="6">
-        <v>10</v>
-      </c>
       <c r="AH13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AI13" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ13" s="6">
-        <v>10</v>
-      </c>
-      <c r="AK13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL13" s="6"/>
-      <c r="AM13" s="6"/>
-      <c r="AN13" s="6"/>
-      <c r="AO13" s="6"/>
+      <c r="AI13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK13" s="6">
+        <v>10</v>
+      </c>
+      <c r="AL13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM13" s="6">
+        <v>10</v>
+      </c>
+      <c r="AN13" s="6">
+        <v>10</v>
+      </c>
+      <c r="AO13" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="AP13" s="6"/>
       <c r="AQ13" s="6"/>
+      <c r="AR13" s="6"/>
+      <c r="AS13" s="6"/>
+      <c r="AT13" s="6"/>
+      <c r="AU13" s="6"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B14" s="16">
         <v>44138</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="6">
+        <f>ROUND(L14/(K14-N14) * 100,2)</f>
+        <v>91.97</v>
+      </c>
+      <c r="F14" s="6">
+        <f>ROUND((P14/(K14-(O14+N14)))*100,2)</f>
+        <v>81.540000000000006</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0.98409999999999997</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="I14" s="6">
+        <v>511</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="K14" s="6">
+        <v>3630</v>
+      </c>
+      <c r="L14" s="6">
+        <v>3266</v>
+      </c>
+      <c r="M14" s="6">
+        <v>285</v>
+      </c>
+      <c r="N14" s="6">
+        <v>79</v>
+      </c>
+      <c r="O14" s="6">
+        <v>2191</v>
+      </c>
+      <c r="P14" s="6">
+        <v>1109</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>251</v>
+      </c>
+      <c r="R14" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="S14" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E14" s="9">
-        <v>0.81540000000000001</v>
-      </c>
-      <c r="F14" s="9">
-        <v>0.98409999999999997</v>
-      </c>
-      <c r="G14" s="6" t="s">
+      <c r="T14" s="9">
+        <v>0.71540000000000004</v>
+      </c>
+      <c r="U14" s="9">
+        <v>0.90080000000000005</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="W14" s="6">
+        <v>10</v>
+      </c>
+      <c r="X14" s="6">
+        <v>75</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z14" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="H14" s="6">
-        <v>511</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="J14" s="6">
-        <v>3630</v>
-      </c>
-      <c r="K14" s="6">
-        <v>3266</v>
-      </c>
-      <c r="L14" s="6">
-        <v>285</v>
-      </c>
-      <c r="M14" s="6">
-        <v>79</v>
-      </c>
-      <c r="N14" s="6" t="s">
+      <c r="AA14" s="9">
+        <v>0.71540000000000004</v>
+      </c>
+      <c r="AB14" s="9">
+        <v>0.93</v>
+      </c>
+      <c r="AC14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD14" s="10">
+        <v>10</v>
+      </c>
+      <c r="AE14" s="10">
+        <v>81</v>
+      </c>
+      <c r="AF14" t="s">
         <v>160</v>
       </c>
-      <c r="O14" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="P14" s="9">
-        <v>0.71540000000000004</v>
-      </c>
-      <c r="Q14" s="9">
-        <v>0.90080000000000005</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="S14" s="6">
-        <v>10</v>
-      </c>
-      <c r="T14" s="6">
-        <v>75</v>
-      </c>
-      <c r="U14" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="V14" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="W14" s="9">
-        <v>0.71540000000000004</v>
-      </c>
-      <c r="X14" s="9">
-        <v>0.93</v>
-      </c>
-      <c r="Y14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z14" s="10">
-        <v>10</v>
-      </c>
-      <c r="AA14" s="10">
-        <v>81</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>164</v>
-      </c>
-      <c r="AC14" s="6" t="s">
+      <c r="AG14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AD14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG14" s="6">
-        <v>10</v>
-      </c>
       <c r="AH14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AI14" s="6">
-        <v>10</v>
-      </c>
-      <c r="AJ14" s="6">
-        <v>10</v>
-      </c>
-      <c r="AK14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL14" s="6"/>
-      <c r="AM14" s="6"/>
-      <c r="AN14" s="6"/>
-      <c r="AO14" s="6"/>
+      <c r="AI14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK14" s="6">
+        <v>10</v>
+      </c>
+      <c r="AL14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM14" s="6">
+        <v>10</v>
+      </c>
+      <c r="AN14" s="6">
+        <v>10</v>
+      </c>
+      <c r="AO14" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="AP14" s="6"/>
       <c r="AQ14" s="6"/>
+      <c r="AR14" s="6"/>
+      <c r="AS14" s="6"/>
+      <c r="AT14" s="6"/>
+      <c r="AU14" s="6"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="Z15" s="10"/>
-      <c r="AA15" s="10"/>
-      <c r="AB15"/>
-      <c r="AC15" s="6"/>
-      <c r="AD15" s="6"/>
-      <c r="AE15" s="6"/>
-      <c r="AF15" s="6"/>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="B15" s="16"/>
+      <c r="C15" s="15"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="10"/>
       <c r="AG15" s="6"/>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
@@ -3152,17 +3408,17 @@
       <c r="AO15" s="6"/>
       <c r="AP15" s="6"/>
       <c r="AQ15" s="6"/>
+      <c r="AR15" s="6"/>
+      <c r="AS15" s="6"/>
+      <c r="AT15" s="6"/>
+      <c r="AU15" s="6"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
-      <c r="AB16"/>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="6"/>
-      <c r="AE16" s="6"/>
-      <c r="AF16" s="6"/>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="F16" s="9"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="AD16" s="10"/>
+      <c r="AE16" s="10"/>
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
@@ -3174,17 +3430,17 @@
       <c r="AO16" s="6"/>
       <c r="AP16" s="6"/>
       <c r="AQ16" s="6"/>
+      <c r="AR16" s="6"/>
+      <c r="AS16" s="6"/>
+      <c r="AT16" s="6"/>
+      <c r="AU16" s="6"/>
     </row>
-    <row r="17" spans="5:43" x14ac:dyDescent="0.3">
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="Z17" s="10"/>
-      <c r="AA17" s="10"/>
-      <c r="AB17"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="6"/>
-      <c r="AE17" s="6"/>
-      <c r="AF17" s="6"/>
+    <row r="17" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="F17" s="9"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="AD17" s="10"/>
+      <c r="AE17" s="10"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
@@ -3196,17 +3452,17 @@
       <c r="AO17" s="6"/>
       <c r="AP17" s="6"/>
       <c r="AQ17" s="6"/>
+      <c r="AR17" s="6"/>
+      <c r="AS17" s="6"/>
+      <c r="AT17" s="6"/>
+      <c r="AU17" s="6"/>
     </row>
-    <row r="18" spans="5:43" x14ac:dyDescent="0.3">
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="Z18" s="10"/>
-      <c r="AA18" s="10"/>
-      <c r="AB18"/>
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="6"/>
-      <c r="AE18" s="6"/>
-      <c r="AF18" s="6"/>
+    <row r="18" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="F18" s="9"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="AD18" s="10"/>
+      <c r="AE18" s="10"/>
       <c r="AG18" s="6"/>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
@@ -3218,17 +3474,17 @@
       <c r="AO18" s="6"/>
       <c r="AP18" s="6"/>
       <c r="AQ18" s="6"/>
+      <c r="AR18" s="6"/>
+      <c r="AS18" s="6"/>
+      <c r="AT18" s="6"/>
+      <c r="AU18" s="6"/>
     </row>
-    <row r="19" spans="5:43" x14ac:dyDescent="0.3">
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="Z19" s="10"/>
-      <c r="AA19" s="10"/>
-      <c r="AB19"/>
-      <c r="AC19" s="6"/>
-      <c r="AD19" s="6"/>
-      <c r="AE19" s="6"/>
-      <c r="AF19" s="6"/>
+    <row r="19" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="F19" s="9"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="10"/>
       <c r="AG19" s="6"/>
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
@@ -3240,17 +3496,17 @@
       <c r="AO19" s="6"/>
       <c r="AP19" s="6"/>
       <c r="AQ19" s="6"/>
+      <c r="AR19" s="6"/>
+      <c r="AS19" s="6"/>
+      <c r="AT19" s="6"/>
+      <c r="AU19" s="6"/>
     </row>
-    <row r="20" spans="5:43" x14ac:dyDescent="0.3">
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="Z20" s="10"/>
-      <c r="AA20" s="10"/>
-      <c r="AB20"/>
-      <c r="AC20" s="6"/>
-      <c r="AD20" s="6"/>
-      <c r="AE20" s="6"/>
-      <c r="AF20" s="6"/>
+    <row r="20" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="F20" s="11"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="AD20" s="10"/>
+      <c r="AE20" s="10"/>
       <c r="AG20" s="6"/>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
@@ -3262,17 +3518,17 @@
       <c r="AO20" s="6"/>
       <c r="AP20" s="6"/>
       <c r="AQ20" s="6"/>
+      <c r="AR20" s="6"/>
+      <c r="AS20" s="6"/>
+      <c r="AT20" s="6"/>
+      <c r="AU20" s="6"/>
     </row>
-    <row r="21" spans="5:43" x14ac:dyDescent="0.3">
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="Z21" s="10"/>
-      <c r="AA21" s="10"/>
-      <c r="AB21"/>
-      <c r="AC21" s="6"/>
-      <c r="AD21" s="6"/>
-      <c r="AE21" s="6"/>
-      <c r="AF21" s="6"/>
+    <row r="21" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="F21" s="9"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="AD21" s="10"/>
+      <c r="AE21" s="10"/>
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
@@ -3284,17 +3540,17 @@
       <c r="AO21" s="6"/>
       <c r="AP21" s="6"/>
       <c r="AQ21" s="6"/>
+      <c r="AR21" s="6"/>
+      <c r="AS21" s="6"/>
+      <c r="AT21" s="6"/>
+      <c r="AU21" s="6"/>
     </row>
-    <row r="22" spans="5:43" x14ac:dyDescent="0.3">
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="Z22" s="10"/>
-      <c r="AA22" s="10"/>
-      <c r="AB22"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="6"/>
-      <c r="AE22" s="6"/>
-      <c r="AF22" s="6"/>
+    <row r="22" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="F22" s="9"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="AD22" s="10"/>
+      <c r="AE22" s="10"/>
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
@@ -3306,17 +3562,17 @@
       <c r="AO22" s="6"/>
       <c r="AP22" s="6"/>
       <c r="AQ22" s="6"/>
+      <c r="AR22" s="6"/>
+      <c r="AS22" s="6"/>
+      <c r="AT22" s="6"/>
+      <c r="AU22" s="6"/>
     </row>
-    <row r="23" spans="5:43" x14ac:dyDescent="0.3">
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="Z23" s="10"/>
-      <c r="AA23" s="10"/>
-      <c r="AB23"/>
-      <c r="AC23" s="6"/>
-      <c r="AD23" s="6"/>
-      <c r="AE23" s="6"/>
-      <c r="AF23" s="6"/>
+    <row r="23" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="F23" s="9"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="AD23" s="10"/>
+      <c r="AE23" s="10"/>
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
@@ -3328,19 +3584,45 @@
       <c r="AO23" s="6"/>
       <c r="AP23" s="6"/>
       <c r="AQ23" s="6"/>
+      <c r="AR23" s="6"/>
+      <c r="AS23" s="6"/>
+      <c r="AT23" s="6"/>
+      <c r="AU23" s="6"/>
     </row>
-    <row r="24" spans="5:43" x14ac:dyDescent="0.3">
-      <c r="E24" s="6" t="s">
-        <v>165</v>
-      </c>
+    <row r="24" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="F24" s="9"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="10"/>
+      <c r="X24"/>
+      <c r="AF24" s="6"/>
+    </row>
+    <row r="25" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="U28" s="10"/>
+      <c r="V28"/>
+      <c r="W28" s="6"/>
+      <c r="AE28"/>
+    </row>
+    <row r="29" spans="6:47" x14ac:dyDescent="0.3">
+      <c r="U29" s="10"/>
+      <c r="V29"/>
+      <c r="W29" s="6"/>
+      <c r="AE29"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="N1:T1"/>
-    <mergeCell ref="U1:AA1"/>
-    <mergeCell ref="AB1:AK1"/>
-    <mergeCell ref="AL1:AQ1"/>
+  <mergeCells count="4">
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:AE1"/>
+    <mergeCell ref="AF1:AO1"/>
+    <mergeCell ref="AP1:AU1"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Added milliseconds time and corrected a reporitng error
</commit_message>
<xml_diff>
--- a/experiments/AlgoComparisons.xlsx
+++ b/experiments/AlgoComparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\mutode_research\newDD\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1349D752-E61D-4CF5-8B65-F5B20304D1DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9069156B-9AC3-476E-ADCE-57010EABDCD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="759" yWindow="759" windowWidth="18851" windowHeight="9845" xr2:uid="{1807BA8C-4E5D-4B92-917C-C9945C819F91}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{1807BA8C-4E5D-4B92-917C-C9945C819F91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="221">
   <si>
     <t>ddMin</t>
   </si>
@@ -415,9 +415,6 @@
     <t>4,9,11,18,22,23,27,29,33,39,40,48,51,52,57,58,62,70,81,82,90,93,95,97,99,100,110,118,122,250,256,260,262,264,265,272,273,274,308,314,328,332,353,356,380,397,402,404,405,413,434,435,437,438,439,443,457,471,472,473,481,489,492</t>
   </si>
   <si>
-    <t>215m</t>
-  </si>
-  <si>
     <t>251ms</t>
   </si>
   <si>
@@ -566,12 +563,156 @@
   </si>
   <si>
     <t>Updated Mutation Score</t>
+  </si>
+  <si>
+    <t>winston@3.3.3</t>
+  </si>
+  <si>
+    <t>5h 25m</t>
+  </si>
+  <si>
+    <t>0-169</t>
+  </si>
+  <si>
+    <t>44s</t>
+  </si>
+  <si>
+    <t>51ms</t>
+  </si>
+  <si>
+    <t>23,62,82,84</t>
+  </si>
+  <si>
+    <t>17,144,62,80</t>
+  </si>
+  <si>
+    <t>85ms</t>
+  </si>
+  <si>
+    <t>96ms</t>
+  </si>
+  <si>
+    <t>163ms</t>
+  </si>
+  <si>
+    <t>OriginalTestSuiteRunningTime (ms)</t>
+  </si>
+  <si>
+    <t>1000ms</t>
+  </si>
+  <si>
+    <t>5000ms</t>
+  </si>
+  <si>
+    <t>10ms</t>
+  </si>
+  <si>
+    <t>3000ms</t>
+  </si>
+  <si>
+    <t>6000ms</t>
+  </si>
+  <si>
+    <t>4000ms</t>
+  </si>
+  <si>
+    <t>2000ms</t>
+  </si>
+  <si>
+    <t>18000ms</t>
+  </si>
+  <si>
+    <t>44000ms</t>
+  </si>
+  <si>
+    <t>42ms</t>
+  </si>
+  <si>
+    <t>178ms</t>
+  </si>
+  <si>
+    <t>25194ms</t>
+  </si>
+  <si>
+    <t>5ms</t>
+  </si>
+  <si>
+    <t>813ms</t>
+  </si>
+  <si>
+    <t>18784ms</t>
+  </si>
+  <si>
+    <t>1227ms</t>
+  </si>
+  <si>
+    <t>13655ms</t>
+  </si>
+  <si>
+    <t>3856ms</t>
+  </si>
+  <si>
+    <t>11ms</t>
+  </si>
+  <si>
+    <t>9ms</t>
+  </si>
+  <si>
+    <t>215ms</t>
+  </si>
+  <si>
+    <t>18ms</t>
+  </si>
+  <si>
+    <t>357ms</t>
+  </si>
+  <si>
+    <t>6ms</t>
+  </si>
+  <si>
+    <t>7ms</t>
+  </si>
+  <si>
+    <t>249ms</t>
+  </si>
+  <si>
+    <t>3357ms</t>
+  </si>
+  <si>
+    <t>2967ms</t>
+  </si>
+  <si>
+    <t>1140ms</t>
+  </si>
+  <si>
+    <t>AlgorithmRunningTime(ms)</t>
+  </si>
+  <si>
+    <t>ReducedTestSuiteRunningTime(ms)</t>
+  </si>
+  <si>
+    <t>36ms</t>
+  </si>
+  <si>
+    <t>14ms</t>
+  </si>
+  <si>
+    <t>3ms</t>
+  </si>
+  <si>
+    <t>172ms</t>
+  </si>
+  <si>
+    <t>429ms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -826,7 +967,6 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -834,6 +974,14 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -843,17 +991,12 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Accent2" xfId="7" builtinId="33"/>
@@ -866,7 +1009,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1" xfId="5" xr:uid="{F4E56029-7EE9-453F-ADCF-12C8305BF6E8}"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="59">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -911,6 +1060,15 @@
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -933,6 +1091,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1121,84 +1282,91 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{952538F1-7DF3-4D7D-A8CC-BE4F7FA56AC6}" name="Table8" displayName="Table8" ref="R2:X23" totalsRowShown="0" headerRowDxfId="52" tableBorderDxfId="51" headerRowCellStyle="Explanatory Text">
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{12B54DEA-7254-4D41-BEC3-BEA4C9B5FD2B}" name="AlgorithmRunningTime" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{C041EDEE-7D1D-40B4-A76F-BE7D7A036172}" name="Reduced Subset" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{2D65E345-C673-4CC1-939C-6D0BF18353C1}" name="Mutation Score" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{4CC4BD8C-4EF4-43AB-BAAB-4E7F5B7FD70D}" name="Coverage" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{644740EE-5F30-46BC-A81B-59EA94F094F2}" name="ReducedTestSuiteRunningTime" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{6C008CB6-3003-451B-83F5-7A2E2094A09F}" name="Tolerance" dataDxfId="45"/>
-    <tableColumn id="7" xr3:uid="{D105531A-8670-4AD8-BDF7-70ED045D32AA}" name="ReducedTestSuiteSize" dataDxfId="44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{952538F1-7DF3-4D7D-A8CC-BE4F7FA56AC6}" name="Table8" displayName="Table8" ref="S2:AA23" totalsRowShown="0" headerRowDxfId="58" tableBorderDxfId="57" headerRowCellStyle="Explanatory Text">
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{12B54DEA-7254-4D41-BEC3-BEA4C9B5FD2B}" name="AlgorithmRunningTime" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{FD2589E2-024E-4F68-81F7-20733BE993EF}" name="AlgorithmRunningTime(ms)" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{C041EDEE-7D1D-40B4-A76F-BE7D7A036172}" name="Reduced Subset" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{2D65E345-C673-4CC1-939C-6D0BF18353C1}" name="Mutation Score" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{4CC4BD8C-4EF4-43AB-BAAB-4E7F5B7FD70D}" name="Coverage" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{644740EE-5F30-46BC-A81B-59EA94F094F2}" name="ReducedTestSuiteRunningTime" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{926B23EE-EA71-4739-B697-5FDE6A0F7B5E}" name="ReducedTestSuiteRunningTime(ms)" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{6C008CB6-3003-451B-83F5-7A2E2094A09F}" name="Tolerance" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{D105531A-8670-4AD8-BDF7-70ED045D32AA}" name="ReducedTestSuiteSize" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{14F4EC92-7BFE-403F-A3C6-CD427D010934}" name="Table9" displayName="Table9" ref="Y2:AE23" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41" headerRowCellStyle="Explanatory Text">
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6C9C0781-48E2-4FB7-8744-C1EDD4F95DCB}" name="AlgorithmRunningTime" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{DA4A4864-0763-4B71-A651-ED4CA4A414F2}" name="Reduced Subset" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{0303DEB1-3A97-457B-8F0B-075435BD2CA4}" name="Mutation Score" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{37441378-B4C1-4801-8946-B5F26FB1A9B8}" name="Coverage" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{5676F7B9-8FF9-49ED-8633-08C2401FF4B2}" name="ReducedTestSuiteRunningTime" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{7E74752D-6DE1-4C73-B537-CFA8D85EDF85}" name="Tolerance" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{2D9D7CF3-D3B4-464C-B1F1-62F1441FBB67}" name="TestSuite Size" dataDxfId="34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{14F4EC92-7BFE-403F-A3C6-CD427D010934}" name="Table9" displayName="Table9" ref="AB2:AJ23" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" tableBorderDxfId="47" headerRowCellStyle="Explanatory Text">
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{6C9C0781-48E2-4FB7-8744-C1EDD4F95DCB}" name="AlgorithmRunningTime" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{233C5AAE-2D9F-46B0-AFC3-CF6AE079FC48}" name="AlgorithmRunningTime(ms)" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{DA4A4864-0763-4B71-A651-ED4CA4A414F2}" name="Reduced Subset" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{0303DEB1-3A97-457B-8F0B-075435BD2CA4}" name="Mutation Score" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{37441378-B4C1-4801-8946-B5F26FB1A9B8}" name="Coverage" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{5676F7B9-8FF9-49ED-8633-08C2401FF4B2}" name="ReducedTestSuiteRunningTime" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{9F03E3C1-CCB7-4996-BB8E-783215C5876D}" name="ReducedTestSuiteRunningTime(ms)" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{7E74752D-6DE1-4C73-B537-CFA8D85EDF85}" name="Tolerance" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{2D9D7CF3-D3B4-464C-B1F1-62F1441FBB67}" name="TestSuite Size" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{21AC0CEF-D177-4D66-B441-7618BEEDE8E3}" name="Table10" displayName="Table10" ref="AF2:AO23" totalsRowShown="0" headerRowDxfId="33" tableBorderDxfId="32" headerRowCellStyle="Explanatory Text">
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{21AC0CEF-D177-4D66-B441-7618BEEDE8E3}" name="Table10" displayName="Table10" ref="AK2:AV23" totalsRowShown="0" headerRowDxfId="39" tableBorderDxfId="38" headerRowCellStyle="Explanatory Text">
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{9B95FA3B-E111-47B3-9FEB-6E34F77C693F}" name="AlgorithmRunningTime"/>
-    <tableColumn id="2" xr3:uid="{CE31A1F2-CCFB-41B9-802E-E4E7D6C22363}" name="Reduced Subset" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{C3588D6B-9C88-46A6-AD70-75921A04F317}" name="Mutation Score" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{640DAF15-6CE5-424F-B23B-0356D0396E43}" name="Coverage" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{72017D7E-EB7B-455E-8490-433A112AD377}" name="ReducedTestSuiteRunningTime" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{2495EE0C-328B-4914-946A-3D5B24547ED9}" name="Starting Tolerance" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{42E4F09C-725B-46FD-8BC3-921A3329D1A6}" name="ToleranceThatFoundASet" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{8E19AD31-C6CB-4914-89F0-9353B6A7CD33}" name="TotalRuns" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{DB462F9A-ABEA-418C-81ED-46797C03550C}" name="ExecutedRuns" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{59135B1B-35D4-4DDB-B9C3-6D510C325029}" name="TestSuite Size" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{AF7FE721-6DCD-4433-B323-4A8DE15712BF}" name="AlgorithmRunningTime(ms)"/>
+    <tableColumn id="2" xr3:uid="{CE31A1F2-CCFB-41B9-802E-E4E7D6C22363}" name="Reduced Subset" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{C3588D6B-9C88-46A6-AD70-75921A04F317}" name="Mutation Score" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{640DAF15-6CE5-424F-B23B-0356D0396E43}" name="Coverage" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{72017D7E-EB7B-455E-8490-433A112AD377}" name="ReducedTestSuiteRunningTime" dataDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{659DABDB-CBE2-4F45-A08D-FC7CCB2AE1B2}" name="ReducedTestSuiteRunningTime(ms)" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{2495EE0C-328B-4914-946A-3D5B24547ED9}" name="Starting Tolerance" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{42E4F09C-725B-46FD-8BC3-921A3329D1A6}" name="ToleranceThatFoundASet" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{8E19AD31-C6CB-4914-89F0-9353B6A7CD33}" name="TotalRuns" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{DB462F9A-ABEA-418C-81ED-46797C03550C}" name="ExecutedRuns" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{59135B1B-35D4-4DDB-B9C3-6D510C325029}" name="TestSuite Size" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{750652E7-E767-41D1-9927-FDCE55E1E6D0}" name="Table12" displayName="Table12" ref="D1:Q29" totalsRowShown="0" headerRowDxfId="22" headerRowCellStyle="Neutral">
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{15CF07D5-B71B-4A28-8125-12ACDB9CC697}" name="Original Set" dataDxfId="21"/>
-    <tableColumn id="15" xr3:uid="{8040B8DD-BF4F-4AF5-9E6F-31B248E7BD01}" name="Original Mutation Score" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{0D187438-7867-4CF4-BC39-4C5405F1DE55}" name="Updated Mutation Score" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{3699F74C-ECE0-4B26-9682-8D573AD734B8}" name="Coverage" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{CD2ECBD2-6A54-4B63-8B16-769F2F08101F}" name="OriginalTestSuiteRunningTime" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{1D29439A-E95C-4EAB-9C6A-44F1FBC75F33}" name="Orignal TestSuite Size" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{1ED35EFA-8CCC-4F74-B0BA-63D0F2B0C067}" name="Mutode Running Time" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{B31DCAD0-6793-4E02-937E-37FDBF007C2A}" name="Orignal Mutants Generated" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{1D18328C-BCA6-4FAC-B58B-4BBF7D4449EA}" name="Original Mutants Killed" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{6EED791C-77AD-4042-BF9C-F7480F2D4091}" name="Original Mutants Survived" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{E3E0C4FE-273D-4C62-984B-F580EF6C1842}" name="Orginal  Mutants Discarded" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{6DF9451B-7D78-466A-B72A-F85A75EAEC85}" name="More Mutants Discarded" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{BB220918-6952-4D3F-8B3B-9016EA4A46E0}" name="Updated Killed Mutants" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{B04458F3-7CA1-40EA-8E87-222BB12FE8D9}" name="Updated Survived Mutant" dataDxfId="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{750652E7-E767-41D1-9927-FDCE55E1E6D0}" name="Table12" displayName="Table12" ref="D1:R29" totalsRowShown="0" headerRowDxfId="28" headerRowCellStyle="Neutral">
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{15CF07D5-B71B-4A28-8125-12ACDB9CC697}" name="Original Set" dataDxfId="27"/>
+    <tableColumn id="15" xr3:uid="{8040B8DD-BF4F-4AF5-9E6F-31B248E7BD01}" name="Original Mutation Score" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{0D187438-7867-4CF4-BC39-4C5405F1DE55}" name="Updated Mutation Score" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{3699F74C-ECE0-4B26-9682-8D573AD734B8}" name="Coverage" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{CD2ECBD2-6A54-4B63-8B16-769F2F08101F}" name="OriginalTestSuiteRunningTime" dataDxfId="23"/>
+    <tableColumn id="16" xr3:uid="{5981330F-249E-45DA-B806-84A900539DB5}" name="OriginalTestSuiteRunningTime (ms)" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{1D29439A-E95C-4EAB-9C6A-44F1FBC75F33}" name="Orignal TestSuite Size" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{1ED35EFA-8CCC-4F74-B0BA-63D0F2B0C067}" name="Mutode Running Time" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{B31DCAD0-6793-4E02-937E-37FDBF007C2A}" name="Orignal Mutants Generated" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{1D18328C-BCA6-4FAC-B58B-4BBF7D4449EA}" name="Original Mutants Killed" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{6EED791C-77AD-4042-BF9C-F7480F2D4091}" name="Original Mutants Survived" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{E3E0C4FE-273D-4C62-984B-F580EF6C1842}" name="Orginal  Mutants Discarded" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{6DF9451B-7D78-466A-B72A-F85A75EAEC85}" name="More Mutants Discarded" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{BB220918-6952-4D3F-8B3B-9016EA4A46E0}" name="Updated Killed Mutants" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{B04458F3-7CA1-40EA-8E87-222BB12FE8D9}" name="Updated Survived Mutant" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0109829-D30D-42C3-9E57-90E25F812D9E}" name="Table2" displayName="Table2" ref="AP2:AU23" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0109829-D30D-42C3-9E57-90E25F812D9E}" name="Table2" displayName="Table2" ref="AW2:BB23" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12" headerRowCellStyle="Accent2">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E4B25968-3AB6-460C-BC4A-98BCD3ED878C}" name="AlgorithmRunningTime" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{3DDDEECD-8312-4190-AA68-6A4E84D065A9}" name="Features to be selected" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{6FD36AEB-1C1B-4058-AE87-EA5A28CA5C75}" name="Reduced Subset" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{F3703558-BD53-4188-AEE9-6233EB063F72}" name="Mutation Score" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{4D7349A3-5B31-4CC5-A72F-4B706196187A}" name="Coverage" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{ED760C3C-7A39-4043-B686-87F211ABDA26}" name="ReducedTestSuiteRunningTime" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{E4B25968-3AB6-460C-BC4A-98BCD3ED878C}" name="AlgorithmRunningTime" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{3DDDEECD-8312-4190-AA68-6A4E84D065A9}" name="Features to be selected" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{6FD36AEB-1C1B-4058-AE87-EA5A28CA5C75}" name="Reduced Subset" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{F3703558-BD53-4188-AEE9-6233EB063F72}" name="Mutation Score" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{4D7349A3-5B31-4CC5-A72F-4B706196187A}" name="Coverage" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{ED760C3C-7A39-4043-B686-87F211ABDA26}" name="ReducedTestSuiteRunningTime" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1501,10 +1669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A84B95-A035-4AC9-8702-F9EE4E2D8975}">
-  <dimension ref="A1:AU29"/>
+  <dimension ref="A1:BB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AS12" sqref="AS12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1541,31 +1709,31 @@
     <col min="31" max="31" width="14.33203125" style="6" customWidth="1"/>
     <col min="32" max="34" width="8.88671875" customWidth="1"/>
     <col min="35" max="35" width="15.5546875" customWidth="1"/>
-    <col min="36" max="37" width="24.6640625" customWidth="1"/>
-    <col min="38" max="38" width="22" customWidth="1"/>
-    <col min="39" max="39" width="23.44140625" customWidth="1"/>
-    <col min="40" max="40" width="20.88671875" customWidth="1"/>
-    <col min="41" max="41" width="34.6640625" customWidth="1"/>
+    <col min="36" max="38" width="24.6640625" customWidth="1"/>
+    <col min="39" max="39" width="22" customWidth="1"/>
+    <col min="40" max="40" width="23.44140625" customWidth="1"/>
+    <col min="41" max="41" width="20.88671875" customWidth="1"/>
+    <col min="42" max="43" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="3" customFormat="1" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:54" s="3" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>6</v>
@@ -1573,14 +1741,14 @@
       <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>164</v>
       </c>
       <c r="L1" s="12" t="s">
         <v>163</v>
@@ -1592,63 +1760,72 @@
         <v>161</v>
       </c>
       <c r="O1" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q1" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="Q1" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="20" t="s">
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="21" t="s">
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
-      <c r="AK1" s="21"/>
-      <c r="AL1" s="21"/>
-      <c r="AM1" s="21"/>
-      <c r="AN1" s="21"/>
-      <c r="AO1" s="21"/>
-      <c r="AP1" s="22" t="s">
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="24"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
+      <c r="AW1" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="AQ1" s="22"/>
-      <c r="AR1" s="22"/>
-      <c r="AS1" s="22"/>
-      <c r="AT1" s="22"/>
-      <c r="AU1" s="22"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
+      <c r="BB1" s="26"/>
     </row>
-    <row r="2" spans="1:47" s="1" customFormat="1" ht="20.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+    <row r="2" spans="1:54" s="1" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="F2" s="24" t="s">
+      <c r="E2" s="19" t="s">
         <v>171</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1658,119 +1835,138 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-      <c r="O2" s="23" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="R2" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="Q2" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AH2" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="AI2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AK2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AL2" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="AM2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AI2" s="8" t="s">
+      <c r="AO2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AJ2" s="8" t="s">
+      <c r="AP2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AQ2" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="AR2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AL2" s="8" t="s">
+      <c r="AS2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="AM2" s="8" t="s">
+      <c r="AT2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AN2" s="8" t="s">
+      <c r="AU2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AO2" s="8" t="s">
+      <c r="AV2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AP2" s="13" t="s">
+      <c r="AW2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="AQ2" s="14" t="s">
+      <c r="AX2" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="AR2" s="14" t="s">
+      <c r="AY2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="AS2" s="14" t="s">
+      <c r="AZ2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AT2" s="14" t="s">
+      <c r="BA2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="AU2" s="14" t="s">
+      <c r="BB2" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="C3" s="25" t="s">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="C3" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="6">
-        <f>ROUND(L3/(K3-N3) * 100,2)</f>
+        <f t="shared" ref="E3:E15" si="0">ROUND(M3/(L3-O3) * 100,2)</f>
         <v>92.83</v>
       </c>
       <c r="F3" s="6">
-        <f>ROUND((P3/(K3-(O3+N3)))*100,2)</f>
+        <f t="shared" ref="F3:F15" si="1">ROUND((Q3/(L3-(P3+O3)))*100,2)</f>
         <v>92.77</v>
       </c>
       <c r="G3" s="9">
@@ -1779,137 +1975,158 @@
       <c r="H3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="6">
         <v>17</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="K3" s="6">
+      <c r="L3" s="6">
         <v>2891</v>
       </c>
-      <c r="L3" s="6">
+      <c r="M3" s="6">
         <v>2666</v>
       </c>
-      <c r="M3" s="6">
+      <c r="N3" s="6">
         <v>206</v>
       </c>
-      <c r="N3" s="6">
+      <c r="O3" s="6">
         <v>19</v>
       </c>
-      <c r="O3" s="6">
+      <c r="P3" s="6">
         <v>22</v>
       </c>
-      <c r="P3" s="6">
+      <c r="Q3" s="6">
         <v>2644</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="R3" s="6">
         <v>206</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="9">
+      <c r="V3" s="9">
         <v>0.85160000000000002</v>
       </c>
-      <c r="U3" s="9">
+      <c r="W3" s="9">
         <v>0.71699999999999997</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="W3" s="6">
-        <v>10</v>
-      </c>
-      <c r="X3" s="6">
+      <c r="Y3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA3" s="6">
         <v>2</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="9">
+      <c r="AE3" s="9">
         <v>0.85160000000000002</v>
       </c>
-      <c r="AB3" s="9">
+      <c r="AF3" s="9">
         <v>0.71699999999999997</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AG3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="AD3" s="10">
-        <v>10</v>
-      </c>
-      <c r="AE3" s="10">
+      <c r="AH3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI3" s="10">
+        <v>10</v>
+      </c>
+      <c r="AJ3" s="10">
         <v>2</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AK3" t="s">
         <v>47</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AL3" t="s">
+        <v>216</v>
+      </c>
+      <c r="AM3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AH3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK3" s="6">
-        <v>10</v>
-      </c>
-      <c r="AL3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM3" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN3" s="6">
-        <v>10</v>
+      <c r="AN3" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="AO3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="AP3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR3" s="6">
+        <v>10</v>
+      </c>
+      <c r="AS3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT3" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU3" s="6">
+        <v>10</v>
+      </c>
+      <c r="AV3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AQ3" s="6">
+      <c r="AX3" s="6">
         <v>8</v>
       </c>
-      <c r="AR3" s="6" t="s">
+      <c r="AY3" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="AS3" s="9">
+      <c r="AZ3" s="9">
         <v>0.92559999999999998</v>
       </c>
-      <c r="AT3" s="9">
+      <c r="BA3" s="9">
         <v>0.91410000000000002</v>
       </c>
-      <c r="AU3" s="6" t="s">
+      <c r="BB3" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="C4" s="25" t="s">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="C4" s="20" t="s">
         <v>55</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="6">
-        <f>ROUND(L4/(K4-N4) * 100,2)</f>
+        <f t="shared" si="0"/>
         <v>8.33</v>
       </c>
       <c r="F4" s="6">
-        <f>ROUND((P4/(K4-(O4+N4)))*100,2)</f>
+        <f t="shared" si="1"/>
         <v>3.68</v>
       </c>
       <c r="G4" s="9">
@@ -1918,137 +2135,158 @@
       <c r="H4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="6">
         <v>4</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="K4" s="6">
+      <c r="L4" s="6">
         <v>1300</v>
       </c>
-      <c r="L4" s="6">
+      <c r="M4" s="6">
         <v>107</v>
       </c>
-      <c r="M4" s="6">
+      <c r="N4" s="6">
         <v>1177</v>
       </c>
-      <c r="N4" s="6">
+      <c r="O4" s="6">
         <v>16</v>
       </c>
-      <c r="O4" s="6">
+      <c r="P4" s="6">
         <v>62</v>
       </c>
-      <c r="P4" s="6">
+      <c r="Q4" s="6">
         <v>45</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="R4" s="6">
         <v>1177</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="S4" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="S4" s="6">
+      <c r="T4" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="U4" s="6">
         <v>3</v>
       </c>
-      <c r="T4" s="9">
+      <c r="V4" s="9">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="U4" s="9">
+      <c r="W4" s="9">
         <v>0.43330000000000002</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="X4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="W4" s="6">
-        <v>10</v>
-      </c>
-      <c r="X4" s="6">
+      <c r="Y4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="6">
         <v>1</v>
       </c>
-      <c r="Y4" s="6" t="s">
+      <c r="AB4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="Z4" s="6">
+      <c r="AC4" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="AD4" s="6">
         <v>3</v>
       </c>
-      <c r="AA4" s="9">
+      <c r="AE4" s="9">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="AB4" s="9">
+      <c r="AF4" s="9">
         <v>0.69610000000000005</v>
       </c>
-      <c r="AC4" s="6" t="s">
+      <c r="AG4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AD4" s="10">
+      <c r="AH4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI4" s="10">
         <v>1</v>
       </c>
-      <c r="AE4" s="10">
+      <c r="AJ4" s="10">
         <v>1</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AK4" t="s">
         <v>48</v>
       </c>
-      <c r="AG4" s="6">
+      <c r="AL4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AM4" s="6">
         <v>0</v>
       </c>
-      <c r="AH4" s="11">
+      <c r="AN4" s="11">
         <v>0</v>
       </c>
-      <c r="AI4" s="9">
+      <c r="AO4" s="9">
         <v>0.48070000000000002</v>
       </c>
-      <c r="AJ4" s="6" t="s">
+      <c r="AP4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AK4" s="6">
+      <c r="AQ4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR4" s="6">
         <v>1</v>
       </c>
-      <c r="AL4" s="6">
+      <c r="AS4" s="6">
         <v>3.68</v>
       </c>
-      <c r="AM4" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN4" s="6">
+      <c r="AT4" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU4" s="6">
         <v>2</v>
       </c>
-      <c r="AO4" s="6">
+      <c r="AV4" s="6">
         <v>1</v>
       </c>
-      <c r="AP4" s="6" t="s">
+      <c r="AW4" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="AQ4" s="6">
+      <c r="AX4" s="6">
         <v>2</v>
       </c>
-      <c r="AR4" s="6" t="s">
+      <c r="AY4" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="AS4" s="9">
+      <c r="AZ4" s="9">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="AT4" s="11">
+      <c r="BA4" s="11">
         <v>0.68</v>
       </c>
-      <c r="AU4" s="11" t="s">
+      <c r="BB4" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="C5" s="25" t="s">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="C5" s="20" t="s">
         <v>56</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="6">
-        <f>ROUND(L5/(K5-N5) * 100,2)</f>
+        <f t="shared" si="0"/>
         <v>89.09</v>
       </c>
       <c r="F5" s="6">
-        <f>ROUND((P5/(K5-(O5+N5)))*100,2)</f>
+        <f t="shared" si="1"/>
         <v>74.41</v>
       </c>
       <c r="G5" s="9">
@@ -2057,138 +2295,159 @@
       <c r="H5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="J5" s="6">
         <v>218</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="K5" s="6">
+      <c r="L5" s="6">
         <v>976</v>
       </c>
-      <c r="L5" s="6">
+      <c r="M5" s="6">
         <v>792</v>
       </c>
-      <c r="M5" s="6">
+      <c r="N5" s="6">
         <v>201</v>
       </c>
-      <c r="N5" s="6">
+      <c r="O5" s="6">
         <v>87</v>
       </c>
-      <c r="O5" s="6">
+      <c r="P5" s="6">
         <v>170</v>
       </c>
-      <c r="P5" s="6">
+      <c r="Q5" s="6">
         <v>535</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="R5" s="6">
         <v>184</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="S5" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="T5" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="U5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T5" s="9">
+      <c r="V5" s="9">
         <v>0.64529999999999998</v>
       </c>
-      <c r="U5" s="9">
+      <c r="W5" s="9">
         <v>0.88549999999999995</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="X5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="W5" s="6">
-        <v>10</v>
-      </c>
-      <c r="X5" s="6">
+      <c r="Y5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA5" s="6">
         <v>42</v>
       </c>
-      <c r="Y5" s="6" t="s">
+      <c r="AB5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Z5" s="6" t="s">
+      <c r="AC5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AA5" s="9">
+      <c r="AE5" s="9">
         <v>0.64529999999999998</v>
       </c>
-      <c r="AB5" s="9">
+      <c r="AF5" s="9">
         <v>0.89159999999999995</v>
       </c>
-      <c r="AC5" s="6" t="s">
+      <c r="AG5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AD5" s="10">
-        <v>10</v>
-      </c>
-      <c r="AE5" s="10">
+      <c r="AH5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI5" s="10">
+        <v>10</v>
+      </c>
+      <c r="AJ5" s="10">
         <v>40</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AK5" t="s">
         <v>49</v>
       </c>
-      <c r="AG5" s="6" t="s">
+      <c r="AL5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AM5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AH5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK5" s="6">
-        <v>10</v>
-      </c>
-      <c r="AL5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM5" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN5" s="6">
-        <v>10</v>
+      <c r="AN5" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="AO5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="AP5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR5" s="6">
+        <v>10</v>
+      </c>
+      <c r="AS5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT5" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU5" s="6">
+        <v>10</v>
+      </c>
+      <c r="AV5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW5" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="AQ5" s="6">
+      <c r="AX5" s="6">
         <v>109</v>
       </c>
-      <c r="AR5" s="6" t="s">
+      <c r="AY5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="AS5" s="9">
+      <c r="AZ5" s="9">
         <v>0.47149999999999997</v>
       </c>
-      <c r="AT5" s="9">
+      <c r="BA5" s="9">
         <v>0.86729999999999996</v>
       </c>
-      <c r="AU5" s="6" t="s">
+      <c r="BB5" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="C6" s="25" t="s">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="C6" s="20" t="s">
         <v>57</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E6" s="6">
-        <f>ROUND(L6/(K6-N6) * 100,2)</f>
+        <f t="shared" si="0"/>
         <v>77.209999999999994</v>
       </c>
       <c r="F6" s="6">
-        <f>ROUND((P6/(K6-(O6+N6)))*100,2)</f>
-        <v>73.25</v>
+        <f t="shared" si="1"/>
+        <v>73.22</v>
       </c>
       <c r="G6" s="9">
         <v>0.98629999999999995</v>
@@ -2196,137 +2455,158 @@
       <c r="H6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J6" s="6">
         <v>858</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K6" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="K6" s="6">
+      <c r="L6" s="6">
         <v>3900</v>
       </c>
-      <c r="L6" s="6">
+      <c r="M6" s="6">
         <v>2483</v>
       </c>
-      <c r="M6" s="6">
+      <c r="N6" s="6">
         <v>733</v>
       </c>
-      <c r="N6" s="6">
+      <c r="O6" s="6">
         <v>684</v>
       </c>
-      <c r="O6" s="6">
-        <v>480</v>
-      </c>
       <c r="P6" s="6">
+        <v>479</v>
+      </c>
+      <c r="Q6" s="6">
         <v>2004</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="R6" s="6">
         <v>733</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="S6" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="T6" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="U6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="9">
+      <c r="V6" s="9">
         <v>0.63239999999999996</v>
       </c>
-      <c r="U6" s="9">
+      <c r="W6" s="9">
         <v>0.82330000000000003</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="X6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="W6" s="6">
-        <v>10</v>
-      </c>
-      <c r="X6" s="6">
+      <c r="Y6" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA6" s="6">
         <v>156</v>
       </c>
-      <c r="Y6" s="6" t="s">
+      <c r="AB6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="Z6" s="9" t="s">
+      <c r="AC6" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="AD6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AA6" s="9">
+      <c r="AE6" s="9">
         <v>0.63239999999999996</v>
       </c>
-      <c r="AB6" s="9">
+      <c r="AF6" s="9">
         <v>0.85670000000000002</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AG6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AD6" s="10">
-        <v>10</v>
-      </c>
-      <c r="AE6" s="10">
+      <c r="AH6" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI6" s="10">
+        <v>10</v>
+      </c>
+      <c r="AJ6" s="10">
         <v>144</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AK6" t="s">
         <v>50</v>
       </c>
-      <c r="AG6" s="6" t="s">
+      <c r="AL6" t="s">
+        <v>207</v>
+      </c>
+      <c r="AM6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AH6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK6" s="6">
-        <v>10</v>
-      </c>
-      <c r="AL6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM6" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN6" s="6">
-        <v>10</v>
+      <c r="AN6" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="AO6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="AP6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR6" s="6">
+        <v>10</v>
+      </c>
+      <c r="AS6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT6" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU6" s="6">
+        <v>10</v>
+      </c>
+      <c r="AV6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW6" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="AQ6" s="6">
+      <c r="AX6" s="6">
         <v>200</v>
       </c>
-      <c r="AR6" s="6" t="s">
+      <c r="AY6" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="AS6" s="9">
+      <c r="AZ6" s="9">
         <v>0.29409999999999997</v>
       </c>
-      <c r="AT6" s="9">
+      <c r="BA6" s="9">
         <v>0.71609999999999996</v>
       </c>
-      <c r="AU6" s="6" t="s">
+      <c r="BB6" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="C7" s="25" t="s">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="C7" s="20" t="s">
         <v>74</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>75</v>
       </c>
       <c r="E7" s="6">
-        <f>ROUND(L7/(K7-N7) * 100,2)</f>
+        <f t="shared" si="0"/>
         <v>7.14</v>
       </c>
       <c r="F7" s="6">
-        <f>ROUND((P7/(K7-(O7+N7)))*100,2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G7" s="9">
@@ -2335,137 +2615,158 @@
       <c r="H7" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J7" s="6">
         <v>8</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="K7" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="K7" s="6">
+      <c r="L7" s="6">
         <v>70</v>
       </c>
-      <c r="L7" s="6">
+      <c r="M7" s="6">
         <v>5</v>
       </c>
-      <c r="M7" s="6">
+      <c r="N7" s="6">
         <v>65</v>
       </c>
-      <c r="N7" s="6">
+      <c r="O7" s="6">
         <v>0</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="6">
         <v>5</v>
       </c>
-      <c r="P7" s="6">
+      <c r="Q7" s="6">
         <v>0</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="R7" s="6">
         <v>65</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="S7" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="S7" s="6">
+      <c r="T7" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="U7" s="6">
         <v>7</v>
       </c>
-      <c r="T7" s="11">
+      <c r="V7" s="11">
         <v>0</v>
       </c>
-      <c r="U7" s="9">
+      <c r="W7" s="9">
         <v>0.79710000000000003</v>
       </c>
-      <c r="V7" s="6" t="s">
+      <c r="X7" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="W7" s="6">
-        <v>10</v>
-      </c>
-      <c r="X7" s="6">
+      <c r="Y7" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA7" s="6">
         <v>1</v>
       </c>
-      <c r="Y7" s="6" t="s">
+      <c r="AB7" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="Z7" s="6" t="s">
+      <c r="AC7" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="AD7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AA7" s="11">
+      <c r="AE7" s="11">
         <v>0</v>
       </c>
-      <c r="AB7" s="11">
+      <c r="AF7" s="11">
         <v>0</v>
       </c>
-      <c r="AC7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD7" s="10">
-        <v>10</v>
-      </c>
-      <c r="AE7" s="10">
+      <c r="AG7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI7" s="10">
+        <v>10</v>
+      </c>
+      <c r="AJ7" s="10">
         <v>0</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AK7" t="s">
         <v>80</v>
       </c>
-      <c r="AG7" s="6" t="s">
+      <c r="AL7" t="s">
+        <v>218</v>
+      </c>
+      <c r="AM7" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AH7" s="11">
+      <c r="AN7" s="11">
         <v>0</v>
       </c>
-      <c r="AI7" s="9">
+      <c r="AO7" s="9">
         <v>0.81159999999999999</v>
       </c>
-      <c r="AJ7" s="6" t="s">
+      <c r="AP7" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AK7" s="6">
-        <v>10</v>
-      </c>
-      <c r="AL7" s="11">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN7" s="6">
-        <v>1</v>
-      </c>
-      <c r="AO7" s="6">
-        <v>7</v>
-      </c>
-      <c r="AP7" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="AQ7" s="6">
-        <v>4</v>
-      </c>
-      <c r="AR7" s="6" t="s">
-        <v>97</v>
+      <c r="AQ7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR7" s="6">
+        <v>10</v>
       </c>
       <c r="AS7" s="11">
         <v>0</v>
       </c>
-      <c r="AT7" s="9">
+      <c r="AT7" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AV7" s="6">
+        <v>7</v>
+      </c>
+      <c r="AW7" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AX7" s="6">
+        <v>4</v>
+      </c>
+      <c r="AY7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ7" s="11">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="9">
         <v>0.57450000000000001</v>
       </c>
-      <c r="AU7" s="6" t="s">
+      <c r="BB7" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="C8" s="25" t="s">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="C8" s="20" t="s">
         <v>58</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E8" s="6">
-        <f>ROUND(L8/(K8-N8) * 100,2)</f>
+        <f t="shared" si="0"/>
         <v>11.59</v>
       </c>
       <c r="F8" s="6">
-        <f>ROUND((P8/(K8-(O8+N8)))*100,2)</f>
+        <f t="shared" si="1"/>
         <v>5.16</v>
       </c>
       <c r="G8" s="9">
@@ -2474,137 +2775,158 @@
       <c r="H8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="6">
         <v>3</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="K8" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="K8" s="6">
+      <c r="L8" s="6">
         <v>814</v>
       </c>
-      <c r="L8" s="6">
+      <c r="M8" s="6">
         <v>94</v>
       </c>
-      <c r="M8" s="6">
+      <c r="N8" s="6">
         <v>717</v>
       </c>
-      <c r="N8" s="6">
+      <c r="O8" s="6">
         <v>3</v>
       </c>
-      <c r="O8" s="6">
+      <c r="P8" s="6">
         <v>55</v>
       </c>
-      <c r="P8" s="6">
+      <c r="Q8" s="6">
         <v>39</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="R8" s="6">
         <v>717</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="S8" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="S8" s="6">
+      <c r="T8" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="U8" s="6">
         <v>2</v>
       </c>
-      <c r="T8" s="9">
+      <c r="V8" s="9">
         <v>5.16E-2</v>
       </c>
-      <c r="U8" s="9">
+      <c r="W8" s="9">
         <v>0.60529999999999995</v>
       </c>
-      <c r="V8" s="6" t="s">
+      <c r="X8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="W8" s="6">
-        <v>10</v>
-      </c>
-      <c r="X8" s="6">
+      <c r="Y8" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z8" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA8" s="6">
         <v>1</v>
       </c>
-      <c r="Y8" s="6" t="s">
+      <c r="AB8" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="Z8" s="6">
+      <c r="AC8" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="AD8" s="6">
         <v>2</v>
       </c>
-      <c r="AA8" s="9">
+      <c r="AE8" s="9">
         <v>5.16E-2</v>
       </c>
-      <c r="AB8" s="9">
+      <c r="AF8" s="9">
         <v>0.60529999999999995</v>
       </c>
-      <c r="AC8" s="6" t="s">
+      <c r="AG8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AD8" s="10">
+      <c r="AH8" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AI8" s="10">
         <v>1</v>
       </c>
-      <c r="AE8" s="10">
+      <c r="AJ8" s="10">
         <v>1</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AK8" t="s">
         <v>63</v>
       </c>
-      <c r="AG8" s="6" t="s">
+      <c r="AL8" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM8" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AH8" s="11">
+      <c r="AN8" s="11">
         <v>0</v>
       </c>
-      <c r="AI8" s="11">
+      <c r="AO8" s="11">
         <v>0</v>
       </c>
-      <c r="AJ8" s="6" t="s">
+      <c r="AP8" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AK8" s="6">
+      <c r="AQ8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR8" s="6">
         <v>1</v>
-      </c>
-      <c r="AL8" s="9">
-        <v>5.16E-2</v>
-      </c>
-      <c r="AM8" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN8" s="6">
-        <v>2</v>
-      </c>
-      <c r="AO8" s="6">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="AQ8" s="6">
-        <v>1</v>
-      </c>
-      <c r="AR8" s="6">
-        <v>2</v>
       </c>
       <c r="AS8" s="9">
         <v>5.16E-2</v>
       </c>
-      <c r="AT8" s="9">
+      <c r="AT8" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU8" s="6">
+        <v>2</v>
+      </c>
+      <c r="AV8" s="6">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX8" s="6">
+        <v>1</v>
+      </c>
+      <c r="AY8" s="6">
+        <v>2</v>
+      </c>
+      <c r="AZ8" s="9">
+        <v>5.16E-2</v>
+      </c>
+      <c r="BA8" s="9">
         <v>0.60529999999999995</v>
       </c>
-      <c r="AU8" s="6" t="s">
+      <c r="BB8" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="C9" s="25" t="s">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="C9" s="20" t="s">
         <v>66</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E9" s="6">
-        <f>ROUND(L9/(K9-N9) * 100,2)</f>
+        <f t="shared" si="0"/>
         <v>81.7</v>
       </c>
       <c r="F9" s="6">
-        <f>ROUND((P9/(K9-(O9+N9)))*100,2)</f>
+        <f t="shared" si="1"/>
         <v>77.38</v>
       </c>
       <c r="G9" s="11">
@@ -2613,137 +2935,158 @@
       <c r="H9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J9" s="6">
         <v>204</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="K9" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="K9" s="6">
+      <c r="L9" s="6">
         <v>885</v>
       </c>
-      <c r="L9" s="6">
+      <c r="M9" s="6">
         <v>701</v>
       </c>
-      <c r="M9" s="6">
+      <c r="N9" s="6">
         <v>157</v>
       </c>
-      <c r="N9" s="6">
+      <c r="O9" s="6">
         <v>27</v>
       </c>
-      <c r="O9" s="6">
+      <c r="P9" s="6">
         <v>164</v>
       </c>
-      <c r="P9" s="6">
+      <c r="Q9" s="6">
         <v>537</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="R9" s="6">
         <v>157</v>
       </c>
-      <c r="R9" s="6" t="s">
+      <c r="S9" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="T9" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="U9" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="T9" s="9">
+      <c r="V9" s="9">
         <v>0.6744</v>
       </c>
-      <c r="U9" s="9">
+      <c r="W9" s="9">
         <v>0.89339999999999997</v>
       </c>
-      <c r="V9" s="6" t="s">
+      <c r="X9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="W9" s="6">
-        <v>10</v>
-      </c>
-      <c r="X9" s="6">
+      <c r="Y9" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA9" s="6">
         <v>42</v>
       </c>
-      <c r="Y9" s="6" t="s">
+      <c r="AB9" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="Z9" s="6" t="s">
+      <c r="AC9" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD9" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="AA9" s="9">
+      <c r="AE9" s="9">
         <v>0.6744</v>
       </c>
-      <c r="AB9" s="9">
+      <c r="AF9" s="9">
         <v>0.89659999999999995</v>
       </c>
-      <c r="AC9" s="6" t="s">
+      <c r="AG9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AD9" s="10">
-        <v>10</v>
-      </c>
-      <c r="AE9" s="10">
+      <c r="AH9" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="AI9" s="10">
+        <v>10</v>
+      </c>
+      <c r="AJ9" s="10">
         <v>35</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AK9" t="s">
         <v>73</v>
       </c>
-      <c r="AG9" s="6" t="s">
+      <c r="AL9" t="s">
+        <v>219</v>
+      </c>
+      <c r="AM9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AH9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK9" s="6">
-        <v>10</v>
-      </c>
-      <c r="AL9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM9" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN9" s="6">
-        <v>10</v>
+      <c r="AN9" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="AO9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="AP9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR9" s="6">
+        <v>10</v>
+      </c>
+      <c r="AS9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT9" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU9" s="6">
+        <v>10</v>
+      </c>
+      <c r="AV9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW9" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="AQ9" s="6">
+      <c r="AX9" s="6">
         <v>102</v>
       </c>
-      <c r="AR9" s="6" t="s">
+      <c r="AY9" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="AS9" s="9">
+      <c r="AZ9" s="9">
         <v>0.47120000000000001</v>
       </c>
-      <c r="AT9" s="9">
+      <c r="BA9" s="9">
         <v>0.879</v>
       </c>
-      <c r="AU9" s="6" t="s">
+      <c r="BB9" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="C10" s="25" t="s">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="C10" s="20" t="s">
         <v>83</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>85</v>
       </c>
       <c r="E10" s="6">
-        <f>ROUND(L10/(K10-N10) * 100,2)</f>
+        <f t="shared" si="0"/>
         <v>79.540000000000006</v>
       </c>
       <c r="F10" s="6">
-        <f>ROUND((P10/(K10-(O10+N10)))*100,2)</f>
+        <f t="shared" si="1"/>
         <v>76.19</v>
       </c>
       <c r="G10" s="9">
@@ -2752,140 +3095,161 @@
       <c r="H10" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="J10" s="6">
         <v>833</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="K10" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="K10" s="6">
+      <c r="L10" s="6">
         <v>3788</v>
       </c>
-      <c r="L10" s="6">
+      <c r="M10" s="6">
         <v>2713</v>
       </c>
-      <c r="M10" s="6">
+      <c r="N10" s="6">
         <v>698</v>
       </c>
-      <c r="N10" s="6">
+      <c r="O10" s="6">
         <v>377</v>
       </c>
-      <c r="O10" s="6">
+      <c r="P10" s="6">
         <v>480</v>
       </c>
-      <c r="P10" s="6">
+      <c r="Q10" s="6">
         <v>2233</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="R10" s="6">
         <v>698</v>
       </c>
-      <c r="R10" s="6" t="s">
+      <c r="S10" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="S10" s="6" t="s">
+      <c r="T10" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="U10" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="T10" s="9">
+      <c r="V10" s="9">
         <v>0.66190000000000004</v>
       </c>
-      <c r="U10" s="9">
+      <c r="W10" s="9">
         <v>0.81289999999999996</v>
       </c>
-      <c r="V10" s="6" t="s">
+      <c r="X10" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W10" s="6">
-        <v>10</v>
-      </c>
-      <c r="X10" s="6">
+      <c r="Y10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA10" s="6">
         <v>148</v>
       </c>
-      <c r="Y10" s="6" t="s">
+      <c r="AB10" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="Z10" s="6" t="s">
+      <c r="AC10" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD10" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="AA10" s="9">
+      <c r="AE10" s="9">
         <v>0.66190000000000004</v>
       </c>
-      <c r="AB10" s="9">
+      <c r="AF10" s="9">
         <v>0.84930000000000005</v>
       </c>
-      <c r="AC10" s="6" t="s">
+      <c r="AG10" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AD10" s="10">
-        <v>10</v>
-      </c>
-      <c r="AE10" s="10">
+      <c r="AH10" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="AI10" s="10">
+        <v>10</v>
+      </c>
+      <c r="AJ10" s="10">
         <v>129</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AK10" t="s">
         <v>90</v>
       </c>
-      <c r="AG10" s="6" t="s">
+      <c r="AL10" t="s">
+        <v>220</v>
+      </c>
+      <c r="AM10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AH10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK10" s="6">
-        <v>10</v>
-      </c>
-      <c r="AL10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM10" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN10" s="6">
-        <v>10</v>
+      <c r="AN10" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="AO10" s="6" t="s">
         <v>15</v>
       </c>
       <c r="AP10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR10" s="6">
+        <v>10</v>
+      </c>
+      <c r="AS10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT10" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU10" s="6">
+        <v>10</v>
+      </c>
+      <c r="AV10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW10" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="AQ10" s="6">
+      <c r="AX10" s="6">
         <v>200</v>
       </c>
-      <c r="AR10" s="6" t="s">
+      <c r="AY10" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AS10" s="9">
+      <c r="AZ10" s="9">
         <v>0.35859999999999997</v>
       </c>
-      <c r="AT10" s="9">
+      <c r="BA10" s="9">
         <v>0.70920000000000005</v>
       </c>
-      <c r="AU10" s="6" t="s">
+      <c r="BB10" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="B11" s="16">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="B11" s="15">
         <v>44128</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="21" t="s">
         <v>119</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>120</v>
       </c>
       <c r="E11" s="6">
-        <f>ROUND(L11/(K11-N11) * 100,2)</f>
+        <f t="shared" si="0"/>
         <v>91.04</v>
       </c>
       <c r="F11" s="6">
-        <f>ROUND((P11/(K11-(O11+N11)))*100,2)</f>
+        <f t="shared" si="1"/>
         <v>86.19</v>
       </c>
       <c r="G11" s="9">
@@ -2894,537 +3258,744 @@
       <c r="H11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J11" s="6">
         <v>494</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="K11" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="K11" s="6">
+      <c r="L11" s="6">
         <v>767</v>
       </c>
-      <c r="L11" s="6">
+      <c r="M11" s="6">
         <v>691</v>
       </c>
-      <c r="M11" s="6">
+      <c r="N11" s="6">
         <v>68</v>
       </c>
-      <c r="N11" s="6">
+      <c r="O11" s="6">
         <v>8</v>
       </c>
-      <c r="O11" s="6">
+      <c r="P11" s="6">
         <v>281</v>
       </c>
-      <c r="P11" s="6">
+      <c r="Q11" s="6">
         <v>412</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="R11" s="6">
         <v>66</v>
       </c>
-      <c r="R11" s="6" t="s">
+      <c r="S11" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="S11" s="6" t="s">
+      <c r="T11" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="U11" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="T11" s="9">
+      <c r="V11" s="9">
         <v>0.76359999999999995</v>
       </c>
-      <c r="U11" s="9">
+      <c r="W11" s="9">
         <v>0.95709999999999995</v>
       </c>
-      <c r="V11" s="6" t="s">
+      <c r="X11" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>63</v>
+      </c>
+      <c r="AB11" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="W11" s="6">
-        <v>10</v>
-      </c>
-      <c r="X11" s="6">
-        <v>63</v>
-      </c>
-      <c r="Y11" s="6" t="s">
+      <c r="AC11" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD11" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="Z11" s="6" t="s">
+      <c r="AE11" s="9">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="AF11" s="9">
+        <v>0.95979999999999999</v>
+      </c>
+      <c r="AG11" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="AA11" s="9">
-        <v>0.76359999999999995</v>
-      </c>
-      <c r="AB11" s="9">
-        <v>0.95979999999999999</v>
-      </c>
-      <c r="AC11" s="6" t="s">
+      <c r="AH11" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AI11" s="10">
+        <v>10</v>
+      </c>
+      <c r="AJ11" s="10">
+        <v>67</v>
+      </c>
+      <c r="AK11" t="s">
         <v>127</v>
       </c>
-      <c r="AD11" s="10">
-        <v>10</v>
-      </c>
-      <c r="AE11" s="10">
-        <v>67</v>
-      </c>
-      <c r="AF11" t="s">
+      <c r="AL11" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR11" s="6">
+        <v>10</v>
+      </c>
+      <c r="AS11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT11" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU11" s="6">
+        <v>10</v>
+      </c>
+      <c r="AV11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW11" s="6"/>
+      <c r="AX11" s="6"/>
+      <c r="AY11" s="6"/>
+      <c r="AZ11" s="6"/>
+      <c r="BA11" s="6"/>
+      <c r="BB11" s="6"/>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="B12" s="15">
+        <v>44128</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="AG11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK11" s="6">
-        <v>10</v>
-      </c>
-      <c r="AL11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM11" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN11" s="6">
-        <v>10</v>
-      </c>
-      <c r="AO11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AP11" s="6"/>
-      <c r="AQ11" s="6"/>
-      <c r="AR11" s="6"/>
-      <c r="AS11" s="6"/>
-      <c r="AT11" s="6"/>
-      <c r="AU11" s="6"/>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="B12" s="16">
-        <v>44128</v>
-      </c>
-      <c r="C12" s="26" t="s">
+      <c r="D12" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>130</v>
-      </c>
       <c r="E12" s="6">
-        <f>ROUND(L12/(K12-N12) * 100,2)</f>
+        <f t="shared" si="0"/>
         <v>88.82</v>
       </c>
       <c r="F12" s="6">
-        <f>ROUND((P12/(K12-(O12+N12)))*100,2)</f>
+        <f t="shared" si="1"/>
         <v>87.98</v>
       </c>
       <c r="G12" s="9">
         <v>0.98599999999999999</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J12" s="6">
+        <v>650</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="L12" s="6">
+        <v>2923</v>
+      </c>
+      <c r="M12" s="6">
+        <v>2541</v>
+      </c>
+      <c r="N12" s="6">
+        <v>320</v>
+      </c>
+      <c r="O12" s="6">
+        <v>62</v>
+      </c>
+      <c r="P12" s="6">
+        <v>198</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>2343</v>
+      </c>
+      <c r="R12" s="6">
+        <v>320</v>
+      </c>
+      <c r="S12" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="T12" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="U12" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="V12" s="9">
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="W12" s="9">
+        <v>0.91790000000000005</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y12" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z12" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA12" s="6">
+        <v>138</v>
+      </c>
+      <c r="AB12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC12" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD12" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="I12" s="6">
-        <v>650</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="K12" s="6">
-        <v>2923</v>
-      </c>
-      <c r="L12" s="6">
-        <v>2541</v>
-      </c>
-      <c r="M12" s="6">
-        <v>320</v>
-      </c>
-      <c r="N12" s="6">
-        <v>62</v>
-      </c>
-      <c r="O12" s="6">
-        <v>198</v>
-      </c>
-      <c r="P12" s="6">
-        <v>2343</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>320</v>
-      </c>
-      <c r="R12" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="S12" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="T12" s="9">
+      <c r="AE12" s="9">
         <v>0.77990000000000004</v>
       </c>
-      <c r="U12" s="9">
-        <v>0.91790000000000005</v>
-      </c>
-      <c r="V12" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="W12" s="6">
-        <v>10</v>
-      </c>
-      <c r="X12" s="6">
-        <v>138</v>
-      </c>
-      <c r="Y12" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z12" s="6" t="s">
+      <c r="AF12" s="9">
+        <v>0.94120000000000004</v>
+      </c>
+      <c r="AG12" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="AA12" s="9">
-        <v>0.77990000000000004</v>
-      </c>
-      <c r="AB12" s="9">
-        <v>0.94120000000000004</v>
-      </c>
-      <c r="AC12" s="6" t="s">
+      <c r="AH12" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI12" s="10">
+        <v>10</v>
+      </c>
+      <c r="AJ12" s="10">
+        <v>141</v>
+      </c>
+      <c r="AK12" t="s">
         <v>137</v>
       </c>
-      <c r="AD12" s="10">
-        <v>10</v>
-      </c>
-      <c r="AE12" s="10">
-        <v>141</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>138</v>
-      </c>
-      <c r="AG12" s="6" t="s">
+      <c r="AL12" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AH12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK12" s="6">
-        <v>10</v>
-      </c>
-      <c r="AL12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM12" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN12" s="6">
-        <v>10</v>
+      <c r="AN12" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="AO12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AP12" s="6"/>
-      <c r="AQ12" s="6"/>
-      <c r="AR12" s="6"/>
-      <c r="AS12" s="6"/>
-      <c r="AT12" s="6"/>
-      <c r="AU12" s="6"/>
+      <c r="AP12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR12" s="6">
+        <v>10</v>
+      </c>
+      <c r="AS12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT12" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU12" s="6">
+        <v>10</v>
+      </c>
+      <c r="AV12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW12" s="6"/>
+      <c r="AX12" s="6"/>
+      <c r="AY12" s="6"/>
+      <c r="AZ12" s="6"/>
+      <c r="BA12" s="6"/>
+      <c r="BB12" s="6"/>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="B13" s="16">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="B13" s="15">
         <v>44135</v>
       </c>
-      <c r="C13" s="26" t="s">
-        <v>141</v>
+      <c r="C13" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E13" s="6">
-        <f>ROUND(L13/(K13-N13) * 100,2)</f>
+        <f t="shared" si="0"/>
         <v>66.569999999999993</v>
       </c>
       <c r="F13" s="6">
-        <f>ROUND((P13/(K13-(O13+N13)))*100,2)</f>
+        <f t="shared" si="1"/>
         <v>54.1</v>
       </c>
       <c r="G13" s="9">
         <v>0.94340000000000002</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="I13" s="6">
+        <v>142</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="J13" s="6">
         <v>17</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="K13" s="6">
+      <c r="K13" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="L13" s="6">
         <v>356</v>
       </c>
-      <c r="L13" s="6">
+      <c r="M13" s="6">
         <v>223</v>
       </c>
-      <c r="M13" s="6">
+      <c r="N13" s="6">
         <v>112</v>
       </c>
-      <c r="N13" s="6">
+      <c r="O13" s="6">
         <v>21</v>
       </c>
-      <c r="O13" s="6">
+      <c r="P13" s="6">
         <v>91</v>
       </c>
-      <c r="P13" s="6">
+      <c r="Q13" s="6">
         <v>132</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="R13" s="6">
         <v>112</v>
       </c>
-      <c r="R13" s="6" t="s">
+      <c r="S13" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="T13" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="U13" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="S13" s="6" t="s">
+      <c r="V13" s="9">
+        <v>0.45079999999999998</v>
+      </c>
+      <c r="W13" s="9">
+        <v>0.91510000000000002</v>
+      </c>
+      <c r="X13" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="T13" s="9">
+      <c r="Y13" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>3</v>
+      </c>
+      <c r="AB13" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC13" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AE13" s="9">
         <v>0.45079999999999998</v>
       </c>
-      <c r="U13" s="9">
+      <c r="AF13" s="9">
         <v>0.91510000000000002</v>
       </c>
-      <c r="V13" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="W13" s="6">
-        <v>10</v>
-      </c>
-      <c r="X13" s="6">
+      <c r="AG13" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH13" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI13" s="10">
+        <v>10</v>
+      </c>
+      <c r="AJ13" s="10">
         <v>3</v>
       </c>
-      <c r="Y13" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="Z13" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA13" s="9">
-        <v>0.45079999999999998</v>
-      </c>
-      <c r="AB13" s="9">
-        <v>0.91510000000000002</v>
-      </c>
-      <c r="AC13" s="6" t="s">
+      <c r="AK13" t="s">
         <v>150</v>
       </c>
-      <c r="AD13" s="10">
-        <v>10</v>
-      </c>
-      <c r="AE13" s="10">
-        <v>3</v>
-      </c>
-      <c r="AF13" t="s">
+      <c r="AL13" t="s">
+        <v>150</v>
+      </c>
+      <c r="AM13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR13" s="6">
+        <v>10</v>
+      </c>
+      <c r="AS13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT13" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU13" s="6">
+        <v>10</v>
+      </c>
+      <c r="AV13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW13" s="6"/>
+      <c r="AX13" s="6"/>
+      <c r="AY13" s="6"/>
+      <c r="AZ13" s="6"/>
+      <c r="BA13" s="6"/>
+      <c r="BB13" s="6"/>
+    </row>
+    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="B14" s="15">
+        <v>44138</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="AG13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK13" s="6">
-        <v>10</v>
-      </c>
-      <c r="AL13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM13" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN13" s="6">
-        <v>10</v>
-      </c>
-      <c r="AO13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AP13" s="6"/>
-      <c r="AQ13" s="6"/>
-      <c r="AR13" s="6"/>
-      <c r="AS13" s="6"/>
-      <c r="AT13" s="6"/>
-      <c r="AU13" s="6"/>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="B14" s="16">
-        <v>44138</v>
-      </c>
-      <c r="C14" s="26" t="s">
+      <c r="D14" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>153</v>
-      </c>
       <c r="E14" s="6">
-        <f>ROUND(L14/(K14-N14) * 100,2)</f>
+        <f t="shared" si="0"/>
         <v>91.97</v>
       </c>
       <c r="F14" s="6">
-        <f>ROUND((P14/(K14-(O14+N14)))*100,2)</f>
+        <f t="shared" si="1"/>
         <v>81.540000000000006</v>
       </c>
       <c r="G14" s="9">
         <v>0.98409999999999997</v>
       </c>
       <c r="H14" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="J14" s="6">
+        <v>511</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="L14" s="6">
+        <v>3630</v>
+      </c>
+      <c r="M14" s="6">
+        <v>3266</v>
+      </c>
+      <c r="N14" s="6">
+        <v>285</v>
+      </c>
+      <c r="O14" s="6">
+        <v>79</v>
+      </c>
+      <c r="P14" s="6">
+        <v>2191</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>1109</v>
+      </c>
+      <c r="R14" s="6">
+        <v>251</v>
+      </c>
+      <c r="S14" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="I14" s="6">
-        <v>511</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="K14" s="6">
-        <v>3630</v>
-      </c>
-      <c r="L14" s="6">
-        <v>3266</v>
-      </c>
-      <c r="M14" s="6">
-        <v>285</v>
-      </c>
-      <c r="N14" s="6">
-        <v>79</v>
-      </c>
-      <c r="O14" s="6">
-        <v>2191</v>
-      </c>
-      <c r="P14" s="6">
-        <v>1109</v>
-      </c>
-      <c r="Q14" s="6">
-        <v>251</v>
-      </c>
-      <c r="R14" s="6" t="s">
+      <c r="T14" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="U14" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="S14" s="6" t="s">
+      <c r="V14" s="9">
+        <v>0.71540000000000004</v>
+      </c>
+      <c r="W14" s="9">
+        <v>0.90080000000000005</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z14" s="6">
+        <v>10</v>
+      </c>
+      <c r="AA14" s="6">
+        <v>75</v>
+      </c>
+      <c r="AB14" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="T14" s="9">
+      <c r="AC14" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE14" s="9">
         <v>0.71540000000000004</v>
       </c>
-      <c r="U14" s="9">
-        <v>0.90080000000000005</v>
-      </c>
-      <c r="V14" s="6" t="s">
+      <c r="AF14" s="9">
+        <v>0.93</v>
+      </c>
+      <c r="AG14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH14" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI14" s="10">
+        <v>10</v>
+      </c>
+      <c r="AJ14" s="10">
+        <v>81</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>159</v>
+      </c>
+      <c r="AM14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR14" s="6">
+        <v>10</v>
+      </c>
+      <c r="AS14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT14" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU14" s="6">
+        <v>10</v>
+      </c>
+      <c r="AV14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW14" s="6"/>
+      <c r="AX14" s="6"/>
+      <c r="AY14" s="6"/>
+      <c r="AZ14" s="6"/>
+      <c r="BA14" s="6"/>
+      <c r="BB14" s="6"/>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="B15" s="15">
+        <v>44146</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="0"/>
+        <v>12.99</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="1"/>
+        <v>6.73</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0.70009999999999994</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="J15" s="6">
+        <v>170</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="L15" s="6">
+        <v>2328</v>
+      </c>
+      <c r="M15" s="6">
+        <v>302</v>
+      </c>
+      <c r="N15" s="6">
+        <v>2023</v>
+      </c>
+      <c r="O15" s="6">
+        <v>3</v>
+      </c>
+      <c r="P15" s="6">
+        <v>1909</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>28</v>
+      </c>
+      <c r="R15" s="6">
+        <v>388</v>
+      </c>
+      <c r="S15" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="T15" s="25"/>
+      <c r="U15" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="V15" s="9">
+        <v>5.7700000000000001E-2</v>
+      </c>
+      <c r="W15" s="9">
+        <v>0.37590000000000001</v>
+      </c>
+      <c r="X15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="W14" s="6">
-        <v>10</v>
-      </c>
-      <c r="X14" s="6">
-        <v>75</v>
-      </c>
-      <c r="Y14" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="Z14" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="AA14" s="9">
-        <v>0.71540000000000004</v>
-      </c>
-      <c r="AB14" s="9">
-        <v>0.93</v>
-      </c>
-      <c r="AC14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD14" s="10">
-        <v>10</v>
-      </c>
-      <c r="AE14" s="10">
-        <v>81</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG14" s="6" t="s">
+      <c r="Y15" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z15" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="6">
+        <v>4</v>
+      </c>
+      <c r="AB15" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC15" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="AD15" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="AE15" s="9">
+        <v>5.7700000000000001E-2</v>
+      </c>
+      <c r="AF15" s="9">
+        <v>0.26750000000000002</v>
+      </c>
+      <c r="AG15" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="AH15" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="AI15" s="10">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="10">
+        <v>4</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>182</v>
+      </c>
+      <c r="AM15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AH14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK14" s="6">
-        <v>10</v>
-      </c>
-      <c r="AL14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM14" s="6">
-        <v>10</v>
-      </c>
-      <c r="AN14" s="6">
-        <v>10</v>
-      </c>
-      <c r="AO14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AP14" s="6"/>
-      <c r="AQ14" s="6"/>
-      <c r="AR14" s="6"/>
-      <c r="AS14" s="6"/>
-      <c r="AT14" s="6"/>
-      <c r="AU14" s="6"/>
+      <c r="AN15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR15" s="6">
+        <v>1</v>
+      </c>
+      <c r="AS15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT15" s="6">
+        <v>10</v>
+      </c>
+      <c r="AU15" s="6">
+        <v>3</v>
+      </c>
+      <c r="AV15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW15" s="6"/>
+      <c r="AX15" s="6"/>
+      <c r="AY15" s="6"/>
+      <c r="AZ15" s="6"/>
+      <c r="BA15" s="6"/>
+      <c r="BB15" s="6"/>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="B15" s="16"/>
-      <c r="C15" s="15"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6"/>
-      <c r="AD15" s="10"/>
-      <c r="AE15" s="10"/>
-      <c r="AG15" s="6"/>
-      <c r="AH15" s="6"/>
-      <c r="AI15" s="6"/>
-      <c r="AJ15" s="6"/>
-      <c r="AK15" s="6"/>
-      <c r="AL15" s="6"/>
-      <c r="AM15" s="6"/>
-      <c r="AN15" s="6"/>
-      <c r="AO15" s="6"/>
-      <c r="AP15" s="6"/>
-      <c r="AQ15" s="6"/>
-      <c r="AR15" s="6"/>
-      <c r="AS15" s="6"/>
-      <c r="AT15" s="6"/>
-      <c r="AU15" s="6"/>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
       <c r="F16" s="9"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
-      <c r="AD16" s="10"/>
-      <c r="AE16" s="10"/>
+      <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
-      <c r="AI16" s="6"/>
-      <c r="AJ16" s="6"/>
-      <c r="AK16" s="6"/>
-      <c r="AL16" s="6"/>
+      <c r="AI16" s="10"/>
+      <c r="AJ16" s="10"/>
       <c r="AM16" s="6"/>
       <c r="AN16" s="6"/>
       <c r="AO16" s="6"/>
@@ -3434,19 +4005,23 @@
       <c r="AS16" s="6"/>
       <c r="AT16" s="6"/>
       <c r="AU16" s="6"/>
+      <c r="AV16" s="6"/>
+      <c r="AW16" s="6"/>
+      <c r="AX16" s="6"/>
+      <c r="AY16" s="6"/>
+      <c r="AZ16" s="6"/>
+      <c r="BA16" s="6"/>
+      <c r="BB16" s="6"/>
     </row>
-    <row r="17" spans="6:47" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:54" x14ac:dyDescent="0.3">
       <c r="F17" s="9"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
-      <c r="AD17" s="10"/>
-      <c r="AE17" s="10"/>
+      <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="6"/>
-      <c r="AI17" s="6"/>
-      <c r="AJ17" s="6"/>
-      <c r="AK17" s="6"/>
-      <c r="AL17" s="6"/>
+      <c r="AI17" s="10"/>
+      <c r="AJ17" s="10"/>
       <c r="AM17" s="6"/>
       <c r="AN17" s="6"/>
       <c r="AO17" s="6"/>
@@ -3456,19 +4031,23 @@
       <c r="AS17" s="6"/>
       <c r="AT17" s="6"/>
       <c r="AU17" s="6"/>
+      <c r="AV17" s="6"/>
+      <c r="AW17" s="6"/>
+      <c r="AX17" s="6"/>
+      <c r="AY17" s="6"/>
+      <c r="AZ17" s="6"/>
+      <c r="BA17" s="6"/>
+      <c r="BB17" s="6"/>
     </row>
-    <row r="18" spans="6:47" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:54" x14ac:dyDescent="0.3">
       <c r="F18" s="9"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="10"/>
+      <c r="AF18" s="6"/>
       <c r="AG18" s="6"/>
       <c r="AH18" s="6"/>
-      <c r="AI18" s="6"/>
-      <c r="AJ18" s="6"/>
-      <c r="AK18" s="6"/>
-      <c r="AL18" s="6"/>
+      <c r="AI18" s="10"/>
+      <c r="AJ18" s="10"/>
       <c r="AM18" s="6"/>
       <c r="AN18" s="6"/>
       <c r="AO18" s="6"/>
@@ -3478,19 +4057,23 @@
       <c r="AS18" s="6"/>
       <c r="AT18" s="6"/>
       <c r="AU18" s="6"/>
+      <c r="AV18" s="6"/>
+      <c r="AW18" s="6"/>
+      <c r="AX18" s="6"/>
+      <c r="AY18" s="6"/>
+      <c r="AZ18" s="6"/>
+      <c r="BA18" s="6"/>
+      <c r="BB18" s="6"/>
     </row>
-    <row r="19" spans="6:47" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:54" x14ac:dyDescent="0.3">
       <c r="F19" s="9"/>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
-      <c r="AD19" s="10"/>
-      <c r="AE19" s="10"/>
+      <c r="AF19" s="6"/>
       <c r="AG19" s="6"/>
       <c r="AH19" s="6"/>
-      <c r="AI19" s="6"/>
-      <c r="AJ19" s="6"/>
-      <c r="AK19" s="6"/>
-      <c r="AL19" s="6"/>
+      <c r="AI19" s="10"/>
+      <c r="AJ19" s="10"/>
       <c r="AM19" s="6"/>
       <c r="AN19" s="6"/>
       <c r="AO19" s="6"/>
@@ -3500,19 +4083,23 @@
       <c r="AS19" s="6"/>
       <c r="AT19" s="6"/>
       <c r="AU19" s="6"/>
+      <c r="AV19" s="6"/>
+      <c r="AW19" s="6"/>
+      <c r="AX19" s="6"/>
+      <c r="AY19" s="6"/>
+      <c r="AZ19" s="6"/>
+      <c r="BA19" s="6"/>
+      <c r="BB19" s="6"/>
     </row>
-    <row r="20" spans="6:47" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:54" x14ac:dyDescent="0.3">
       <c r="F20" s="11"/>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
-      <c r="AD20" s="10"/>
-      <c r="AE20" s="10"/>
+      <c r="AF20" s="6"/>
       <c r="AG20" s="6"/>
       <c r="AH20" s="6"/>
-      <c r="AI20" s="6"/>
-      <c r="AJ20" s="6"/>
-      <c r="AK20" s="6"/>
-      <c r="AL20" s="6"/>
+      <c r="AI20" s="10"/>
+      <c r="AJ20" s="10"/>
       <c r="AM20" s="6"/>
       <c r="AN20" s="6"/>
       <c r="AO20" s="6"/>
@@ -3522,19 +4109,23 @@
       <c r="AS20" s="6"/>
       <c r="AT20" s="6"/>
       <c r="AU20" s="6"/>
+      <c r="AV20" s="6"/>
+      <c r="AW20" s="6"/>
+      <c r="AX20" s="6"/>
+      <c r="AY20" s="6"/>
+      <c r="AZ20" s="6"/>
+      <c r="BA20" s="6"/>
+      <c r="BB20" s="6"/>
     </row>
-    <row r="21" spans="6:47" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:54" x14ac:dyDescent="0.3">
       <c r="F21" s="9"/>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
-      <c r="AD21" s="10"/>
-      <c r="AE21" s="10"/>
+      <c r="AF21" s="6"/>
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
-      <c r="AI21" s="6"/>
-      <c r="AJ21" s="6"/>
-      <c r="AK21" s="6"/>
-      <c r="AL21" s="6"/>
+      <c r="AI21" s="10"/>
+      <c r="AJ21" s="10"/>
       <c r="AM21" s="6"/>
       <c r="AN21" s="6"/>
       <c r="AO21" s="6"/>
@@ -3544,19 +4135,23 @@
       <c r="AS21" s="6"/>
       <c r="AT21" s="6"/>
       <c r="AU21" s="6"/>
+      <c r="AV21" s="6"/>
+      <c r="AW21" s="6"/>
+      <c r="AX21" s="6"/>
+      <c r="AY21" s="6"/>
+      <c r="AZ21" s="6"/>
+      <c r="BA21" s="6"/>
+      <c r="BB21" s="6"/>
     </row>
-    <row r="22" spans="6:47" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:54" x14ac:dyDescent="0.3">
       <c r="F22" s="9"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
-      <c r="AD22" s="10"/>
-      <c r="AE22" s="10"/>
+      <c r="AF22" s="6"/>
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
-      <c r="AI22" s="6"/>
-      <c r="AJ22" s="6"/>
-      <c r="AK22" s="6"/>
-      <c r="AL22" s="6"/>
+      <c r="AI22" s="10"/>
+      <c r="AJ22" s="10"/>
       <c r="AM22" s="6"/>
       <c r="AN22" s="6"/>
       <c r="AO22" s="6"/>
@@ -3566,19 +4161,23 @@
       <c r="AS22" s="6"/>
       <c r="AT22" s="6"/>
       <c r="AU22" s="6"/>
+      <c r="AV22" s="6"/>
+      <c r="AW22" s="6"/>
+      <c r="AX22" s="6"/>
+      <c r="AY22" s="6"/>
+      <c r="AZ22" s="6"/>
+      <c r="BA22" s="6"/>
+      <c r="BB22" s="6"/>
     </row>
-    <row r="23" spans="6:47" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:54" x14ac:dyDescent="0.3">
       <c r="F23" s="9"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
-      <c r="AD23" s="10"/>
-      <c r="AE23" s="10"/>
+      <c r="AF23" s="6"/>
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
-      <c r="AI23" s="6"/>
-      <c r="AJ23" s="6"/>
-      <c r="AK23" s="6"/>
-      <c r="AL23" s="6"/>
+      <c r="AI23" s="10"/>
+      <c r="AJ23" s="10"/>
       <c r="AM23" s="6"/>
       <c r="AN23" s="6"/>
       <c r="AO23" s="6"/>
@@ -3588,41 +4187,50 @@
       <c r="AS23" s="6"/>
       <c r="AT23" s="6"/>
       <c r="AU23" s="6"/>
+      <c r="AV23" s="6"/>
+      <c r="AW23" s="6"/>
+      <c r="AX23" s="6"/>
+      <c r="AY23" s="6"/>
+      <c r="AZ23" s="6"/>
+      <c r="BA23" s="6"/>
+      <c r="BB23" s="6"/>
     </row>
-    <row r="24" spans="6:47" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:54" x14ac:dyDescent="0.3">
       <c r="F24" s="9"/>
       <c r="V24" s="6"/>
-      <c r="W24" s="10"/>
-      <c r="X24"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="10"/>
+      <c r="Y24"/>
       <c r="AF24" s="6"/>
+      <c r="AG24" s="6"/>
     </row>
-    <row r="25" spans="6:47" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:54" x14ac:dyDescent="0.3">
       <c r="F25" s="9"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="10"/>
+      <c r="X25"/>
+      <c r="AF25" s="6"/>
     </row>
-    <row r="26" spans="6:47" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:54" x14ac:dyDescent="0.3">
       <c r="F26" s="9"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="10"/>
+      <c r="X26"/>
+      <c r="AF26" s="6"/>
     </row>
-    <row r="27" spans="6:47" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:54" x14ac:dyDescent="0.3">
       <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="6:47" x14ac:dyDescent="0.3">
-      <c r="U28" s="10"/>
-      <c r="V28"/>
-      <c r="W28" s="6"/>
-      <c r="AE28"/>
-    </row>
-    <row r="29" spans="6:47" x14ac:dyDescent="0.3">
-      <c r="U29" s="10"/>
-      <c r="V29"/>
-      <c r="W29" s="6"/>
-      <c r="AE29"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="10"/>
+      <c r="X27"/>
+      <c r="AF27" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:AE1"/>
-    <mergeCell ref="AF1:AO1"/>
-    <mergeCell ref="AP1:AU1"/>
+    <mergeCell ref="AW1:BB1"/>
+    <mergeCell ref="S1:AA1"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="AK1:AV1"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
@@ -3636,15 +4244,16 @@
     <hyperlink ref="C10" r:id="rId8" xr:uid="{2AD2D1E5-BBEF-4677-89E1-016A7A0FAED2}"/>
     <hyperlink ref="C11" r:id="rId9" display="shortid@2.2.16" xr:uid="{B888CDFE-6A23-42E0-8CA1-53F217448B93}"/>
     <hyperlink ref="C14" r:id="rId10" xr:uid="{E399C88D-FCD1-4571-B019-AEF8F40F42C7}"/>
+    <hyperlink ref="C15" r:id="rId11" xr:uid="{253D1FDA-01C1-4D56-9342-15E974766BD2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
   <tableParts count="5">
-    <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
     <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>